<commit_message>
Payment success connect client call and template formula changes for CW CMA
</commit_message>
<xml_diff>
--- a/service-loans/template/Template_CW_CMA.xlsx
+++ b/service-loans/template/Template_CW_CMA.xlsx
@@ -589,8 +589,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -1109,9 +1109,9 @@
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1307,7 +1307,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="43" fontId="3" fillId="6" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1384,7 +1384,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
@@ -1396,7 +1396,7 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection hidden="1"/>
     </xf>
@@ -1482,6 +1482,41 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection hidden="1"/>
@@ -1498,43 +1533,12 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1543,10 +1547,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
   </cellXfs>
@@ -1860,11 +1860,11 @@
   <dimension ref="A1:R86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B41" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B67" sqref="B67"/>
       <selection pane="topRight" activeCell="B67" sqref="B67"/>
       <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3:M3"/>
+      <selection pane="bottomRight" activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -3024,11 +3024,11 @@
         <v>10</v>
       </c>
       <c r="B48" s="28">
-        <f t="shared" ref="B48:M48" si="9">(ROUND(B40+B44+B46-B42,2))</f>
+        <f>(ROUND(B44+B46,2))</f>
         <v>0</v>
       </c>
       <c r="C48" s="28">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="C48:M48" si="9">(ROUND(C44+C46,2))</f>
         <v>0</v>
       </c>
       <c r="D48" s="28">
@@ -3067,7 +3067,7 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="M48" s="29">
+      <c r="M48" s="28">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -4125,7 +4125,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="i7bRWGa+rRvmEZHLTH7dSqE7uEXTSX6elu5SrIJSRqKpbm0MmN+f3mGHKYsFuFm4nig26SI4WHY/wtZY4M8CKA==" saltValue="jzkUdNftsDFr4t5c+u4J7w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="4">
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A1:M1"/>
@@ -4170,70 +4169,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="115" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
-      <c r="D1" s="121"/>
-      <c r="E1" s="121"/>
-      <c r="F1" s="121"/>
-      <c r="G1" s="121"/>
-      <c r="H1" s="121"/>
-      <c r="I1" s="121"/>
-      <c r="J1" s="121"/>
-      <c r="K1" s="121"/>
-      <c r="L1" s="121"/>
-      <c r="M1" s="121"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="115"/>
+      <c r="L1" s="115"/>
+      <c r="M1" s="115"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="122" t="s">
+      <c r="A2" s="116" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="122"/>
-      <c r="C2" s="122"/>
-      <c r="D2" s="122"/>
-      <c r="E2" s="122"/>
-      <c r="F2" s="122"/>
-      <c r="G2" s="122"/>
-      <c r="H2" s="122"/>
-      <c r="I2" s="122"/>
-      <c r="J2" s="122"/>
-      <c r="K2" s="122"/>
-      <c r="L2" s="122"/>
-      <c r="M2" s="122"/>
+      <c r="B2" s="116"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
+      <c r="I2" s="116"/>
+      <c r="J2" s="116"/>
+      <c r="K2" s="116"/>
+      <c r="L2" s="116"/>
+      <c r="M2" s="116"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="123" t="s">
+      <c r="A3" s="117" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="123"/>
-      <c r="C3" s="123"/>
-      <c r="D3" s="123"/>
-      <c r="E3" s="123"/>
-      <c r="F3" s="123"/>
-      <c r="G3" s="123"/>
-      <c r="H3" s="123"/>
-      <c r="I3" s="123"/>
-      <c r="J3" s="123"/>
-      <c r="K3" s="123"/>
-      <c r="L3" s="123"/>
-      <c r="M3" s="123"/>
+      <c r="B3" s="117"/>
+      <c r="C3" s="117"/>
+      <c r="D3" s="117"/>
+      <c r="E3" s="117"/>
+      <c r="F3" s="117"/>
+      <c r="G3" s="117"/>
+      <c r="H3" s="117"/>
+      <c r="I3" s="117"/>
+      <c r="J3" s="117"/>
+      <c r="K3" s="117"/>
+      <c r="L3" s="117"/>
+      <c r="M3" s="117"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="125" t="s">
+      <c r="A4" s="120" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="125"/>
-      <c r="C4" s="125"/>
-      <c r="D4" s="125"/>
-      <c r="E4" s="125"/>
-      <c r="F4" s="125"/>
-      <c r="G4" s="125"/>
-      <c r="H4" s="125"/>
-      <c r="I4" s="125"/>
-      <c r="J4" s="125"/>
-      <c r="K4" s="125"/>
+      <c r="B4" s="120"/>
+      <c r="C4" s="120"/>
+      <c r="D4" s="120"/>
+      <c r="E4" s="120"/>
+      <c r="F4" s="120"/>
+      <c r="G4" s="120"/>
+      <c r="H4" s="120"/>
+      <c r="I4" s="120"/>
+      <c r="J4" s="120"/>
+      <c r="K4" s="120"/>
       <c r="L4" s="1" t="str">
         <f>'Operating Stmt.'!L4</f>
         <v>Rupees</v>
@@ -4244,7 +4243,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="117" t="s">
+      <c r="A5" s="126" t="s">
         <v>72</v>
       </c>
       <c r="B5" s="63">
@@ -4297,70 +4296,70 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="118"/>
-      <c r="B6" s="119" t="str">
+      <c r="A6" s="127"/>
+      <c r="B6" s="118" t="str">
         <f>+'Operating Stmt.'!B6:B6</f>
         <v>Audited</v>
       </c>
-      <c r="C6" s="119" t="str">
+      <c r="C6" s="118" t="str">
         <f>+'Operating Stmt.'!C6:C6</f>
         <v>Audited</v>
       </c>
-      <c r="D6" s="119" t="str">
+      <c r="D6" s="118" t="str">
         <f>+'Operating Stmt.'!D6:D6</f>
         <v>Audited</v>
       </c>
-      <c r="E6" s="119" t="str">
+      <c r="E6" s="118" t="str">
         <f>+'Operating Stmt.'!E6:E6</f>
         <v>Estimated</v>
       </c>
-      <c r="F6" s="119" t="str">
+      <c r="F6" s="118" t="str">
         <f>+'Operating Stmt.'!F6:F6</f>
         <v>Projected</v>
       </c>
-      <c r="G6" s="119" t="str">
+      <c r="G6" s="118" t="str">
         <f>+'Operating Stmt.'!G6:G6</f>
         <v>Projected</v>
       </c>
-      <c r="H6" s="119" t="str">
+      <c r="H6" s="118" t="str">
         <f>+'Operating Stmt.'!H6:H6</f>
         <v>Projected</v>
       </c>
-      <c r="I6" s="119" t="str">
+      <c r="I6" s="118" t="str">
         <f>+'Operating Stmt.'!I6:I6</f>
         <v>Projected</v>
       </c>
-      <c r="J6" s="119" t="str">
+      <c r="J6" s="118" t="str">
         <f>+'Operating Stmt.'!J6:J6</f>
         <v>Projected</v>
       </c>
-      <c r="K6" s="119" t="str">
+      <c r="K6" s="118" t="str">
         <f>+'Operating Stmt.'!K6:K6</f>
         <v>Projected</v>
       </c>
-      <c r="L6" s="119" t="str">
+      <c r="L6" s="118" t="str">
         <f>+'Operating Stmt.'!L6:L6</f>
         <v>Projected</v>
       </c>
-      <c r="M6" s="126" t="str">
+      <c r="M6" s="122" t="str">
         <f>+'Operating Stmt.'!M6:M6</f>
         <v>Projected</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="118"/>
-      <c r="B7" s="124"/>
-      <c r="C7" s="124"/>
-      <c r="D7" s="124"/>
-      <c r="E7" s="124"/>
-      <c r="F7" s="120"/>
-      <c r="G7" s="120"/>
-      <c r="H7" s="120"/>
-      <c r="I7" s="120"/>
-      <c r="J7" s="120"/>
-      <c r="K7" s="120"/>
-      <c r="L7" s="120"/>
-      <c r="M7" s="127"/>
+      <c r="A7" s="127"/>
+      <c r="B7" s="119"/>
+      <c r="C7" s="119"/>
+      <c r="D7" s="119"/>
+      <c r="E7" s="119"/>
+      <c r="F7" s="121"/>
+      <c r="G7" s="121"/>
+      <c r="H7" s="121"/>
+      <c r="I7" s="121"/>
+      <c r="J7" s="121"/>
+      <c r="K7" s="121"/>
+      <c r="L7" s="121"/>
+      <c r="M7" s="123"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="68" t="s">
@@ -4806,7 +4805,7 @@
       <c r="M32" s="11"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="115"/>
+      <c r="A33" s="124"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
       <c r="D33" s="15"/>
@@ -4821,7 +4820,7 @@
       <c r="M33" s="59"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="116"/>
+      <c r="A34" s="125"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
       <c r="D34" s="15"/>
@@ -5983,8 +5982,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="7W+SJ6wMc/O96WhI3y/t2RXMCnY9zOonXIj9VS9vJ2spn71uHgApmPZWW0rChKt8Wa2k03OV1LgCgF222glkaA==" saltValue="OVxbTUYFsa7vvLq/X0zo8w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="18">
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="M6:M7"/>
     <mergeCell ref="A33:A34"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="L6:L7"/>
@@ -6001,6 +5998,8 @@
     <mergeCell ref="K6:K7"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="I6:I7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="M6:M7"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:M13 B17:M32 B82:M83 B41:M53 B67:M80 B57:M57">
@@ -6035,70 +6034,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="115" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
-      <c r="D1" s="121"/>
-      <c r="E1" s="121"/>
-      <c r="F1" s="121"/>
-      <c r="G1" s="121"/>
-      <c r="H1" s="121"/>
-      <c r="I1" s="121"/>
-      <c r="J1" s="121"/>
-      <c r="K1" s="121"/>
-      <c r="L1" s="121"/>
-      <c r="M1" s="121"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="115"/>
+      <c r="L1" s="115"/>
+      <c r="M1" s="115"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="122" t="s">
+      <c r="A2" s="116" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="122"/>
-      <c r="C2" s="122"/>
-      <c r="D2" s="122"/>
-      <c r="E2" s="122"/>
-      <c r="F2" s="122"/>
-      <c r="G2" s="122"/>
-      <c r="H2" s="122"/>
-      <c r="I2" s="122"/>
-      <c r="J2" s="122"/>
-      <c r="K2" s="122"/>
-      <c r="L2" s="122"/>
-      <c r="M2" s="122"/>
+      <c r="B2" s="116"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
+      <c r="I2" s="116"/>
+      <c r="J2" s="116"/>
+      <c r="K2" s="116"/>
+      <c r="L2" s="116"/>
+      <c r="M2" s="116"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="128" t="s">
+      <c r="A3" s="129" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="128"/>
-      <c r="C3" s="128"/>
-      <c r="D3" s="128"/>
-      <c r="E3" s="128"/>
-      <c r="F3" s="128"/>
-      <c r="G3" s="128"/>
-      <c r="H3" s="128"/>
-      <c r="I3" s="128"/>
-      <c r="J3" s="128"/>
-      <c r="K3" s="128"/>
-      <c r="L3" s="128"/>
-      <c r="M3" s="128"/>
+      <c r="B3" s="129"/>
+      <c r="C3" s="129"/>
+      <c r="D3" s="129"/>
+      <c r="E3" s="129"/>
+      <c r="F3" s="129"/>
+      <c r="G3" s="129"/>
+      <c r="H3" s="129"/>
+      <c r="I3" s="129"/>
+      <c r="J3" s="129"/>
+      <c r="K3" s="129"/>
+      <c r="L3" s="129"/>
+      <c r="M3" s="129"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="125" t="s">
+      <c r="A4" s="120" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="125"/>
-      <c r="C4" s="125"/>
-      <c r="D4" s="125"/>
-      <c r="E4" s="125"/>
-      <c r="F4" s="125"/>
-      <c r="G4" s="125"/>
-      <c r="H4" s="125"/>
-      <c r="I4" s="125"/>
-      <c r="J4" s="125"/>
-      <c r="K4" s="125"/>
+      <c r="B4" s="120"/>
+      <c r="C4" s="120"/>
+      <c r="D4" s="120"/>
+      <c r="E4" s="120"/>
+      <c r="F4" s="120"/>
+      <c r="G4" s="120"/>
+      <c r="H4" s="120"/>
+      <c r="I4" s="120"/>
+      <c r="J4" s="120"/>
+      <c r="K4" s="120"/>
       <c r="L4" s="1" t="str">
         <f>'Operating Stmt.'!L4</f>
         <v>Rupees</v>
@@ -6109,7 +6108,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="129" t="s">
+      <c r="A5" s="130" t="s">
         <v>96</v>
       </c>
       <c r="B5" s="96">
@@ -6162,70 +6161,70 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="130"/>
-      <c r="B6" s="119" t="str">
+      <c r="A6" s="131"/>
+      <c r="B6" s="118" t="str">
         <f>Liabilities!B6</f>
         <v>Audited</v>
       </c>
-      <c r="C6" s="119" t="str">
+      <c r="C6" s="118" t="str">
         <f>Liabilities!C6</f>
         <v>Audited</v>
       </c>
-      <c r="D6" s="119" t="str">
+      <c r="D6" s="118" t="str">
         <f>Liabilities!D6</f>
         <v>Audited</v>
       </c>
-      <c r="E6" s="119" t="str">
+      <c r="E6" s="118" t="str">
         <f>Liabilities!E6</f>
         <v>Estimated</v>
       </c>
-      <c r="F6" s="119" t="str">
+      <c r="F6" s="118" t="str">
         <f>Liabilities!F6</f>
         <v>Projected</v>
       </c>
-      <c r="G6" s="119" t="str">
+      <c r="G6" s="118" t="str">
         <f>Liabilities!G6</f>
         <v>Projected</v>
       </c>
-      <c r="H6" s="119" t="str">
+      <c r="H6" s="118" t="str">
         <f>Liabilities!H6</f>
         <v>Projected</v>
       </c>
-      <c r="I6" s="119" t="str">
+      <c r="I6" s="118" t="str">
         <f>Liabilities!I6</f>
         <v>Projected</v>
       </c>
-      <c r="J6" s="119" t="str">
+      <c r="J6" s="118" t="str">
         <f>Liabilities!J6</f>
         <v>Projected</v>
       </c>
-      <c r="K6" s="119" t="str">
+      <c r="K6" s="118" t="str">
         <f>Liabilities!K6</f>
         <v>Projected</v>
       </c>
-      <c r="L6" s="119" t="str">
+      <c r="L6" s="118" t="str">
         <f>Liabilities!L6</f>
         <v>Projected</v>
       </c>
-      <c r="M6" s="126" t="str">
+      <c r="M6" s="122" t="str">
         <f>Liabilities!M6</f>
         <v>Projected</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="130"/>
-      <c r="B7" s="124"/>
-      <c r="C7" s="124"/>
-      <c r="D7" s="124"/>
-      <c r="E7" s="124"/>
-      <c r="F7" s="124"/>
-      <c r="G7" s="124"/>
-      <c r="H7" s="124"/>
-      <c r="I7" s="124"/>
-      <c r="J7" s="124"/>
-      <c r="K7" s="124"/>
-      <c r="L7" s="124"/>
-      <c r="M7" s="131"/>
+      <c r="A7" s="131"/>
+      <c r="B7" s="119"/>
+      <c r="C7" s="119"/>
+      <c r="D7" s="119"/>
+      <c r="E7" s="119"/>
+      <c r="F7" s="119"/>
+      <c r="G7" s="119"/>
+      <c r="H7" s="119"/>
+      <c r="I7" s="119"/>
+      <c r="J7" s="119"/>
+      <c r="K7" s="119"/>
+      <c r="L7" s="119"/>
+      <c r="M7" s="128"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="98" t="s">
@@ -8422,6 +8421,8 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="gCAJhDjH91pGkDLgQzOyLcFfRSAHratKW2iXt0Hxaq6M33QoW20Nxys2xqN7voXArV6XgVCTL9MwusoeDnmfDQ==" saltValue="6OueseyPnOxBOBmcQuv/tg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="17">
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:L7"/>
     <mergeCell ref="M6:M7"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="A2:M2"/>
@@ -8437,8 +8438,6 @@
     <mergeCell ref="H6:H7"/>
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="50" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
npOrgId added in CorporateFinal and Primary view.cw_cma template added.
</commit_message>
<xml_diff>
--- a/service-loans/template/Template_CW_CMA.xlsx
+++ b/service-loans/template/Template_CW_CMA.xlsx
@@ -1551,17 +1551,17 @@
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1884,11 +1884,11 @@
   <dimension ref="A1:R86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B46" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B67" sqref="B67"/>
       <selection pane="topRight" activeCell="B67" sqref="B67"/>
       <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomRight" activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -3047,51 +3047,51 @@
         <v>10</v>
       </c>
       <c r="B48" s="49">
-        <f t="shared" ref="B48:M48" si="9">(ROUND(B40+B44+B46,2))</f>
+        <f>(ROUND(B44+B46,2))</f>
         <v>0</v>
       </c>
       <c r="C48" s="49">
-        <f t="shared" si="9"/>
+        <f>(ROUND(C44+C46,2))</f>
         <v>0</v>
       </c>
       <c r="D48" s="49">
-        <f t="shared" si="9"/>
+        <f>(ROUND(D44+D46,2))</f>
         <v>0</v>
       </c>
       <c r="E48" s="49">
-        <f t="shared" si="9"/>
+        <f>(ROUND(E44+E46,2))</f>
         <v>0</v>
       </c>
       <c r="F48" s="49">
-        <f t="shared" si="9"/>
+        <f>(ROUND(F44+F46,2))</f>
         <v>0</v>
       </c>
       <c r="G48" s="49">
-        <f t="shared" si="9"/>
+        <f>(ROUND(G44+G46,2))</f>
         <v>0</v>
       </c>
       <c r="H48" s="49">
-        <f t="shared" si="9"/>
+        <f>(ROUND(H44+H46,2))</f>
         <v>0</v>
       </c>
       <c r="I48" s="49">
-        <f t="shared" si="9"/>
+        <f>(ROUND(I44+I46,2))</f>
         <v>0</v>
       </c>
       <c r="J48" s="49">
-        <f t="shared" si="9"/>
+        <f>(ROUND(J44+J46,2))</f>
         <v>0</v>
       </c>
       <c r="K48" s="49">
-        <f t="shared" si="9"/>
+        <f>(ROUND(K44+K46,2))</f>
         <v>0</v>
       </c>
       <c r="L48" s="49">
-        <f t="shared" si="9"/>
+        <f>(ROUND(L44+L46,2))</f>
         <v>0</v>
       </c>
       <c r="M48" s="104">
-        <f t="shared" si="9"/>
+        <f>(ROUND(M44+M46,2))</f>
         <v>0</v>
       </c>
     </row>
@@ -3147,51 +3147,51 @@
         <v>8</v>
       </c>
       <c r="B52" s="49">
-        <f t="shared" ref="B52:M52" si="10">(ROUND(B48-B50,2))</f>
+        <f t="shared" ref="B52:M52" si="9">(ROUND(B48-B50,2))</f>
         <v>0</v>
       </c>
       <c r="C52" s="49">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="D52" s="49">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="E52" s="49">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F52" s="49">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G52" s="49">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H52" s="49">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I52" s="49">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J52" s="49">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="K52" s="49">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="L52" s="49">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M52" s="104">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -3283,47 +3283,47 @@
         <v>0</v>
       </c>
       <c r="C58" s="49">
-        <f t="shared" ref="C58:M58" si="11">(ROUND(C52+C56+C54,2))</f>
+        <f t="shared" ref="C58:M58" si="10">(ROUND(C52+C56+C54,2))</f>
         <v>0</v>
       </c>
       <c r="D58" s="49">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="E58" s="49">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F58" s="49">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="G58" s="49">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H58" s="49">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I58" s="49">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J58" s="49">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K58" s="49">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="L58" s="49">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="M58" s="104">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -3347,51 +3347,51 @@
         <v>102</v>
       </c>
       <c r="B60" s="49">
-        <f t="shared" ref="B60:M60" si="12">IF(B58&lt;0,(ROUND(B15+B58,2)),(ROUND(B15-B58,2)))</f>
+        <f t="shared" ref="B60:M60" si="11">IF(B58&lt;0,(ROUND(B15+B58,2)),(ROUND(B15-B58,2)))</f>
         <v>0</v>
       </c>
       <c r="C60" s="49">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="D60" s="49">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="E60" s="49">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F60" s="49">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="G60" s="49">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="H60" s="49">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="I60" s="49">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="J60" s="49">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="K60" s="49">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L60" s="49">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="M60" s="104">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -3447,51 +3447,51 @@
         <v>104</v>
       </c>
       <c r="B64" s="49">
-        <f t="shared" ref="B64:M64" si="13">(ROUND(B60-B62,2))</f>
+        <f t="shared" ref="B64:M64" si="12">(ROUND(B60-B62,2))</f>
         <v>0</v>
       </c>
       <c r="C64" s="49">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="D64" s="49">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="E64" s="49">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="F64" s="49">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="G64" s="49">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="H64" s="49">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I64" s="49">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="J64" s="49">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="K64" s="49">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="L64" s="49">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M64" s="104">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -3532,51 +3532,51 @@
         <v>7</v>
       </c>
       <c r="B67" s="49">
-        <f t="shared" ref="B67:M67" si="14">B66</f>
+        <f t="shared" ref="B67:M67" si="13">B66</f>
         <v>0</v>
       </c>
       <c r="C67" s="49">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="D67" s="49">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="E67" s="49">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="F67" s="49">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="G67" s="49">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H67" s="49">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="I67" s="49">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="J67" s="49">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K67" s="49">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L67" s="49">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="M67" s="104">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -3602,51 +3602,51 @@
         <v>5</v>
       </c>
       <c r="B69" s="49">
-        <f t="shared" ref="B69:M69" si="15">B68</f>
+        <f t="shared" ref="B69:M69" si="14">B68</f>
         <v>0</v>
       </c>
       <c r="C69" s="49">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="D69" s="49">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="E69" s="49">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="F69" s="49">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="G69" s="49">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H69" s="49">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="I69" s="49">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="J69" s="49">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K69" s="49">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="L69" s="49">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M69" s="104">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -3655,51 +3655,51 @@
         <v>4</v>
       </c>
       <c r="B70" s="49">
-        <f t="shared" ref="B70:M70" si="16">SUM(ROUND(B67-B69,2))</f>
+        <f t="shared" ref="B70:M70" si="15">SUM(ROUND(B67-B69,2))</f>
         <v>0</v>
       </c>
       <c r="C70" s="49">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="D70" s="49">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="E70" s="49">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="F70" s="49">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="G70" s="49">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="H70" s="49">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="I70" s="49">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="J70" s="49">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="K70" s="49">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L70" s="49">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="M70" s="104">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -3740,51 +3740,51 @@
         <v>106</v>
       </c>
       <c r="B73" s="49">
-        <f t="shared" ref="B73:M73" si="17">SUM(ROUND(B64+B70-B71,2))</f>
+        <f t="shared" ref="B73:M73" si="16">SUM(ROUND(B64+B70-B71,2))</f>
         <v>0</v>
       </c>
       <c r="C73" s="49">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="D73" s="49">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="E73" s="49">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="F73" s="49">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="G73" s="49">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H73" s="49">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="I73" s="49">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="J73" s="49">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="K73" s="49">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="L73" s="49">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="M73" s="104">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -4031,51 +4031,51 @@
         <v>109</v>
       </c>
       <c r="B84" s="49">
-        <f t="shared" ref="B84:M84" si="18">B78-B80</f>
+        <f t="shared" ref="B84:M84" si="17">B78-B80</f>
         <v>0</v>
       </c>
       <c r="C84" s="49">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="D84" s="49">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="E84" s="49">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="F84" s="49">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="G84" s="49">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="H84" s="49">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="I84" s="49">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="J84" s="49">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="K84" s="49">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="L84" s="49">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="M84" s="104">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -4099,56 +4099,56 @@
         <v>110</v>
       </c>
       <c r="B86" s="50">
-        <f t="shared" ref="B86:M86" si="19">IFERROR((B84/B78),0)</f>
+        <f t="shared" ref="B86:M86" si="18">IFERROR((B84/B78),0)</f>
         <v>0</v>
       </c>
       <c r="C86" s="50">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="D86" s="50">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="E86" s="50">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="F86" s="50">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="G86" s="50">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H86" s="50">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="I86" s="50">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="J86" s="50">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="K86" s="50">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="L86" s="50">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="M86" s="106">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Ruc88LWM6cER4ni9pVxsj4UbvozoxKddwgD0uTSFpV3YF2kbyx3Jz2QA+M2X/j0ds3hKiCglQ/Hn3zQSeembxA==" saltValue="tygsqoCz3+yYXL3LoWA2dw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="BsmTXYPCDduW8uo+x4Wjiog5Usd5Fw35BXK06T+zGQrqfu6Dhv9QF/ynhE3czc3GijSPXYvHmCd+tMN6i2QgIw==" saltValue="efcxZt1rYQuwhgUOcDHT5g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="4">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
@@ -4178,11 +4178,11 @@
   <dimension ref="A1:M87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="7" topLeftCell="B37" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B67" sqref="B67"/>
       <selection pane="topRight" activeCell="B67" sqref="B67"/>
       <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -4237,13 +4237,13 @@
       <c r="M2" s="55"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="129" t="s">
+      <c r="A3" s="127" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="129"/>
-      <c r="C3" s="129"/>
-      <c r="D3" s="129"/>
-      <c r="E3" s="129"/>
+      <c r="B3" s="127"/>
+      <c r="C3" s="127"/>
+      <c r="D3" s="127"/>
+      <c r="E3" s="127"/>
       <c r="F3" s="57"/>
       <c r="G3" s="57"/>
       <c r="H3" s="57"/>
@@ -4379,17 +4379,17 @@
         <f>+'Operating Stmt.'!L6:L6</f>
         <v>Projected</v>
       </c>
-      <c r="M6" s="127" t="str">
+      <c r="M6" s="129" t="str">
         <f>+'Operating Stmt.'!M6:M6</f>
         <v>Projected</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="121"/>
-      <c r="B7" s="130"/>
-      <c r="C7" s="130"/>
-      <c r="D7" s="130"/>
-      <c r="E7" s="130"/>
+      <c r="B7" s="128"/>
+      <c r="C7" s="128"/>
+      <c r="D7" s="128"/>
+      <c r="E7" s="128"/>
       <c r="F7" s="123"/>
       <c r="G7" s="123"/>
       <c r="H7" s="123"/>
@@ -4397,7 +4397,7 @@
       <c r="J7" s="123"/>
       <c r="K7" s="123"/>
       <c r="L7" s="123"/>
-      <c r="M7" s="128"/>
+      <c r="M7" s="130"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="64" t="s">
@@ -4523,15 +4523,15 @@
         <v>66</v>
       </c>
       <c r="B15" s="68">
-        <f t="shared" ref="B15:M15" si="0">SUM(ROUND(B11+B12,2))</f>
+        <f>SUM(ROUND(B11+B12,2))</f>
         <v>0</v>
       </c>
       <c r="C15" s="68">
-        <f t="shared" si="0"/>
+        <f>SUM(ROUND(C11+C12,2))</f>
         <v>0</v>
       </c>
       <c r="D15" s="68">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B15:M15" si="0">SUM(ROUND(D11+D12,2))</f>
         <v>0</v>
       </c>
       <c r="E15" s="68">
@@ -5969,11 +5969,11 @@
         <v>125</v>
       </c>
       <c r="B87" s="82">
-        <f t="shared" ref="B87:M87" si="8">SUM(ROUND(B63+B85,2))</f>
+        <f>SUM(ROUND(B63+B85,2))</f>
         <v>0</v>
       </c>
       <c r="C87" s="82">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="B87:M87" si="8">SUM(ROUND(C63+C85,2))</f>
         <v>0</v>
       </c>
       <c r="D87" s="82">
@@ -6018,7 +6018,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="su+1KEb5AXfIECIVzOpPiutOuFRHIyNTvHyW/wDX1mfT2XFhHgfvmRelYrl5DWJ9HLRVhedCmgmoDxYRqWSbeg==" saltValue="qrXx3jyIE4eY0NF/CGVMqQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Vh3co2K3auc2SO4KXVDI6k1EQx3Ckj3sn5ZcWM7CP3FwOAt2NiBqyHr5mfTr2P1iBb1SFynUH0U95Saz66ioXQ==" saltValue="Hcog5vwf8WANu53WAA84Zg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="18">
     <mergeCell ref="M6:M7"/>
     <mergeCell ref="F6:F7"/>
@@ -6068,7 +6068,7 @@
       <selection activeCell="B67" sqref="B67"/>
       <selection pane="topRight" activeCell="B67" sqref="B67"/>
       <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
-      <selection pane="bottomRight" activeCell="A92" sqref="A92"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -6123,13 +6123,13 @@
       <c r="M2" s="55"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="129" t="s">
+      <c r="A3" s="127" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="129"/>
-      <c r="C3" s="129"/>
-      <c r="D3" s="129"/>
-      <c r="E3" s="129"/>
+      <c r="B3" s="127"/>
+      <c r="C3" s="127"/>
+      <c r="D3" s="127"/>
+      <c r="E3" s="127"/>
       <c r="F3" s="57"/>
       <c r="G3" s="57"/>
       <c r="H3" s="57"/>
@@ -6265,24 +6265,24 @@
         <f>Liabilities!L6</f>
         <v>Projected</v>
       </c>
-      <c r="M6" s="127" t="str">
+      <c r="M6" s="129" t="str">
         <f>Liabilities!M6</f>
         <v>Projected</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="133"/>
-      <c r="B7" s="130"/>
-      <c r="C7" s="130"/>
-      <c r="D7" s="130"/>
-      <c r="E7" s="130"/>
-      <c r="F7" s="130"/>
-      <c r="G7" s="130"/>
-      <c r="H7" s="130"/>
-      <c r="I7" s="130"/>
-      <c r="J7" s="130"/>
-      <c r="K7" s="130"/>
-      <c r="L7" s="130"/>
+      <c r="B7" s="128"/>
+      <c r="C7" s="128"/>
+      <c r="D7" s="128"/>
+      <c r="E7" s="128"/>
+      <c r="F7" s="128"/>
+      <c r="G7" s="128"/>
+      <c r="H7" s="128"/>
+      <c r="I7" s="128"/>
+      <c r="J7" s="128"/>
+      <c r="K7" s="128"/>
+      <c r="L7" s="128"/>
       <c r="M7" s="131"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -8478,12 +8478,8 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="8/JreBCuvHVVvQwIx7bQmCmjhuRvYm9+BN6btFcTR6Vqu0ieM2bpSRlLgKJ2kRt1g5KPOBI55t11ppBiBv0L/A==" saltValue="32zoxFpnnWe0anY93dg+XQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="AjL5mar7wgLPvac6BlJB0XUYC6V5Eqnr3Hb6j84Cb16ksyH4cZ7g1s3iYJ6TJbhMjjIE/eWDZ+odLkYp05QBhg==" saltValue="p3uk3iD0ptTlDDUKr/O9yA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="17">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:C4"/>
     <mergeCell ref="M6:M7"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="B6:B7"/>
@@ -8497,6 +8493,10 @@
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="K6:K7"/>
     <mergeCell ref="L6:L7"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:C4"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4">

</xml_diff>

<commit_message>
remove drop down from excel file
</commit_message>
<xml_diff>
--- a/service-loans/template/Template_CW_CMA.xlsx
+++ b/service-loans/template/Template_CW_CMA.xlsx
@@ -5,7 +5,7 @@
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="nMIDBcyH02QIBA4bXtkulhW+BkwLjO6uUdnHuLe/vey9rIzKWc8NDkCsYZON8UKSky/yikEzYHsiuF6pBe7KDg==" workbookSaltValue="OCFZwCBGKUImSpaXHpKcuQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Operating Stmt." sheetId="2" r:id="rId1"/>
@@ -654,10 +654,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -1216,9 +1216,9 @@
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1258,7 +1258,7 @@
     </xf>
     <xf numFmtId="2" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="43" fontId="3" fillId="6" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1445,10 +1445,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1482,6 +1482,18 @@
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -1493,12 +1505,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1517,12 +1523,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1849,7 +1849,7 @@
       <selection activeCell="B67" sqref="B67"/>
       <selection pane="topRight" activeCell="B67" sqref="B67"/>
       <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1857,10 +1857,10 @@
     <col min="1" max="1" width="51.85546875" style="20" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="5" width="17.7109375" style="20" customWidth="1" collapsed="1"/>
     <col min="6" max="7" width="7.5703125" style="20" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="10" width="9.140625" style="20" hidden="1" collapsed="1"/>
-    <col min="11" max="13" width="0" style="20" hidden="1"/>
-    <col min="14" max="15" width="7.5703125" style="20" hidden="1"/>
-    <col min="16" max="18" width="9.140625" style="20" hidden="1"/>
+    <col min="8" max="10" width="9.140625" style="20" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="13" width="0" style="20" hidden="1" customWidth="1"/>
+    <col min="14" max="15" width="7.5703125" style="20" hidden="1" customWidth="1"/>
+    <col min="16" max="18" width="9.140625" style="20" hidden="1" customWidth="1"/>
     <col min="19" max="16384" width="9.140625" style="20" hidden="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -2881,24 +2881,18 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="43hQJQ+uaU5zsIuQWkFeNt1MC3H/E52Oed7WULemk8PhVtBGrj63ZqPzuUuwmyB8gNBCzUnzN3YbF7wFQ30QXw==" saltValue="8pvodnTfFe6Iqa2tKAL2SQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="CpAPyf8NidhQkA/BL47gJy5l1CTP+p/BpDHjnHiK3JmkxZFbSR1gvjWBtoL7ZFJHSx3sjM+cO2LRHIOBYOLojQ==" saltValue="DWGuAkpal+NwIBjnqqatsQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="4">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="A4:C4"/>
   </mergeCells>
-  <dataValidations count="4">
+  <dataValidations count="2">
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:E16 B18:E81">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82:E86 B17:E17"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4">
-      <formula1>$F$2</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4">
-      <formula1>$F$1:$J$1</formula1>
-    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2927,13 +2921,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="113" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="111"/>
-      <c r="C1" s="111"/>
-      <c r="D1" s="111"/>
-      <c r="E1" s="111"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
       <c r="F1" s="42"/>
       <c r="G1" s="43"/>
       <c r="H1" s="43"/>
@@ -2954,13 +2948,13 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="112" t="s">
+      <c r="A2" s="114" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="112"/>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
+      <c r="B2" s="114"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="114"/>
+      <c r="E2" s="114"/>
       <c r="F2" s="46"/>
       <c r="G2" s="46"/>
       <c r="H2" s="46"/>
@@ -2971,13 +2965,13 @@
       <c r="M2" s="46"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="114" t="s">
+      <c r="A3" s="116" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="114"/>
-      <c r="C3" s="114"/>
-      <c r="D3" s="114"/>
-      <c r="E3" s="114"/>
+      <c r="B3" s="116"/>
+      <c r="C3" s="116"/>
+      <c r="D3" s="116"/>
+      <c r="E3" s="116"/>
       <c r="F3" s="48"/>
       <c r="G3" s="48"/>
       <c r="H3" s="48"/>
@@ -2988,11 +2982,11 @@
       <c r="M3" s="48"/>
     </row>
     <row r="4" spans="1:13" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="113" t="s">
+      <c r="A4" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="113"/>
-      <c r="C4" s="113"/>
+      <c r="B4" s="115"/>
+      <c r="C4" s="115"/>
       <c r="D4" s="21" t="s">
         <v>40</v>
       </c>
@@ -3015,7 +3009,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="107" t="s">
+      <c r="A5" s="111" t="s">
         <v>71</v>
       </c>
       <c r="B5" s="30">
@@ -3068,70 +3062,70 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="108"/>
-      <c r="B6" s="109" t="str">
+      <c r="A6" s="112"/>
+      <c r="B6" s="107" t="str">
         <f>+'Operating Stmt.'!B6:B6</f>
         <v>Audited</v>
       </c>
-      <c r="C6" s="109" t="str">
+      <c r="C6" s="107" t="str">
         <f>+'Operating Stmt.'!C6:C6</f>
         <v>Audited</v>
       </c>
-      <c r="D6" s="109" t="str">
+      <c r="D6" s="107" t="str">
         <f>+'Operating Stmt.'!D6:D6</f>
         <v>Audited</v>
       </c>
-      <c r="E6" s="109" t="str">
+      <c r="E6" s="107" t="str">
         <f>+'Operating Stmt.'!E6:E6</f>
         <v>Estimated</v>
       </c>
-      <c r="F6" s="109" t="e">
+      <c r="F6" s="107" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="G6" s="109" t="e">
+      <c r="G6" s="107" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="H6" s="109" t="e">
+      <c r="H6" s="107" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="I6" s="109" t="e">
+      <c r="I6" s="107" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="J6" s="109" t="e">
+      <c r="J6" s="107" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="109" t="e">
+      <c r="K6" s="107" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="L6" s="109" t="e">
+      <c r="L6" s="107" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="M6" s="116" t="e">
+      <c r="M6" s="105" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="108"/>
-      <c r="B7" s="115"/>
-      <c r="C7" s="115"/>
-      <c r="D7" s="115"/>
-      <c r="E7" s="115"/>
-      <c r="F7" s="110"/>
-      <c r="G7" s="110"/>
-      <c r="H7" s="110"/>
-      <c r="I7" s="110"/>
-      <c r="J7" s="110"/>
-      <c r="K7" s="110"/>
-      <c r="L7" s="110"/>
-      <c r="M7" s="117"/>
+      <c r="A7" s="112"/>
+      <c r="B7" s="117"/>
+      <c r="C7" s="117"/>
+      <c r="D7" s="117"/>
+      <c r="E7" s="117"/>
+      <c r="F7" s="108"/>
+      <c r="G7" s="108"/>
+      <c r="H7" s="108"/>
+      <c r="I7" s="108"/>
+      <c r="J7" s="108"/>
+      <c r="K7" s="108"/>
+      <c r="L7" s="108"/>
+      <c r="M7" s="106"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="55" t="s">
@@ -3577,7 +3571,7 @@
       <c r="M32" s="4"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="105"/>
+      <c r="A33" s="109"/>
       <c r="B33" s="57"/>
       <c r="C33" s="57"/>
       <c r="D33" s="57"/>
@@ -3592,7 +3586,7 @@
       <c r="M33" s="4"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="106"/>
+      <c r="A34" s="110"/>
       <c r="B34" s="57"/>
       <c r="C34" s="57"/>
       <c r="D34" s="57"/>
@@ -4754,14 +4748,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="Fmj0YJ21lQXt9wjgpuGV85vU6k5CC2HVpsj3RzdzaGabq4QO99/nBoyYvjjxeXfxe6mcbqf7YNaypxkcHprMuA==" saltValue="IsolDYy4cpDOrYQdLdHN3A==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="18">
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="H6:H7"/>
     <mergeCell ref="A33:A34"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="A1:E1"/>
@@ -4772,6 +4758,14 @@
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="H6:H7"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:M13 B17:M32 B82:M83 B41:M53 B67:M80 B57:M57">
@@ -4814,13 +4808,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="113" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="111"/>
-      <c r="C1" s="111"/>
-      <c r="D1" s="111"/>
-      <c r="E1" s="111"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
       <c r="F1" s="43"/>
       <c r="G1" s="43"/>
       <c r="H1" s="43"/>
@@ -4841,13 +4835,13 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="112" t="s">
+      <c r="A2" s="114" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="112"/>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
+      <c r="B2" s="114"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="114"/>
+      <c r="E2" s="114"/>
       <c r="F2" s="46"/>
       <c r="G2" s="46"/>
       <c r="H2" s="46"/>
@@ -4858,13 +4852,13 @@
       <c r="M2" s="46"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="114" t="s">
+      <c r="A3" s="116" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="114"/>
-      <c r="C3" s="114"/>
-      <c r="D3" s="114"/>
-      <c r="E3" s="114"/>
+      <c r="B3" s="116"/>
+      <c r="C3" s="116"/>
+      <c r="D3" s="116"/>
+      <c r="E3" s="116"/>
       <c r="F3" s="48"/>
       <c r="G3" s="48"/>
       <c r="H3" s="48"/>
@@ -4875,11 +4869,11 @@
       <c r="M3" s="48"/>
     </row>
     <row r="4" spans="1:13" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="113" t="s">
+      <c r="A4" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="113"/>
-      <c r="C4" s="113"/>
+      <c r="B4" s="115"/>
+      <c r="C4" s="115"/>
       <c r="D4" s="21" t="s">
         <v>40</v>
       </c>
@@ -4956,68 +4950,68 @@
     </row>
     <row r="6" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="120"/>
-      <c r="B6" s="109" t="str">
+      <c r="B6" s="107" t="str">
         <f>Liabilities!B6</f>
         <v>Audited</v>
       </c>
-      <c r="C6" s="109" t="str">
+      <c r="C6" s="107" t="str">
         <f>Liabilities!C6</f>
         <v>Audited</v>
       </c>
-      <c r="D6" s="109" t="str">
+      <c r="D6" s="107" t="str">
         <f>Liabilities!D6</f>
         <v>Audited</v>
       </c>
-      <c r="E6" s="109" t="str">
+      <c r="E6" s="107" t="str">
         <f>Liabilities!E6</f>
         <v>Estimated</v>
       </c>
-      <c r="F6" s="109" t="e">
+      <c r="F6" s="107" t="e">
         <f>Liabilities!F6</f>
         <v>#REF!</v>
       </c>
-      <c r="G6" s="109" t="e">
+      <c r="G6" s="107" t="e">
         <f>Liabilities!G6</f>
         <v>#REF!</v>
       </c>
-      <c r="H6" s="109" t="e">
+      <c r="H6" s="107" t="e">
         <f>Liabilities!H6</f>
         <v>#REF!</v>
       </c>
-      <c r="I6" s="109" t="e">
+      <c r="I6" s="107" t="e">
         <f>Liabilities!I6</f>
         <v>#REF!</v>
       </c>
-      <c r="J6" s="109" t="e">
+      <c r="J6" s="107" t="e">
         <f>Liabilities!J6</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="109" t="e">
+      <c r="K6" s="107" t="e">
         <f>Liabilities!K6</f>
         <v>#REF!</v>
       </c>
-      <c r="L6" s="109" t="e">
+      <c r="L6" s="107" t="e">
         <f>Liabilities!L6</f>
         <v>#REF!</v>
       </c>
-      <c r="M6" s="116" t="e">
+      <c r="M6" s="105" t="e">
         <f>Liabilities!M6</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="120"/>
-      <c r="B7" s="115"/>
-      <c r="C7" s="115"/>
-      <c r="D7" s="115"/>
-      <c r="E7" s="115"/>
-      <c r="F7" s="115"/>
-      <c r="G7" s="115"/>
-      <c r="H7" s="115"/>
-      <c r="I7" s="115"/>
-      <c r="J7" s="115"/>
-      <c r="K7" s="115"/>
-      <c r="L7" s="115"/>
+      <c r="B7" s="117"/>
+      <c r="C7" s="117"/>
+      <c r="D7" s="117"/>
+      <c r="E7" s="117"/>
+      <c r="F7" s="117"/>
+      <c r="G7" s="117"/>
+      <c r="H7" s="117"/>
+      <c r="I7" s="117"/>
+      <c r="J7" s="117"/>
+      <c r="K7" s="117"/>
+      <c r="L7" s="117"/>
       <c r="M7" s="118"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -7215,6 +7209,7 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="rHFnn36dDXVsjiSgK8V7A0sh5cIHrtuty/phCDBmp5QeYFfHehd+M2RumDAvPsSYihnV3DBianORAQokAFfAbw==" saltValue="PuqpZdmDzQ05Ip9IdfgtvQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="17">
+    <mergeCell ref="L6:L7"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A3:E3"/>
@@ -7231,7 +7226,6 @@
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4">

</xml_diff>

<commit_message>
new cma template added gauravbhai.
</commit_message>
<xml_diff>
--- a/service-loans/template/Template_CW_CMA.xlsx
+++ b/service-loans/template/Template_CW_CMA.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="nMIDBcyH02QIBA4bXtkulhW+BkwLjO6uUdnHuLe/vey9rIzKWc8NDkCsYZON8UKSky/yikEzYHsiuF6pBe7KDg==" workbookSaltValue="OCFZwCBGKUImSpaXHpKcuQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Operating Stmt." sheetId="2" r:id="rId1"/>
     <sheet name="Liabilities" sheetId="3" r:id="rId2"/>
     <sheet name="Asset" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="171">
   <si>
     <t xml:space="preserve">     [b] Dividend Rate [in %]</t>
   </si>
@@ -545,16 +545,25 @@
   <si>
     <t>31. Investments [other than long-term investments]</t>
   </si>
+  <si>
+    <t>Other Income: Need to check at the time of Due Diligence</t>
+  </si>
+  <si>
+    <t>Other Liabilities (Need to check at the time of Due Diligence)</t>
+  </si>
+  <si>
+    <t>Other Assets (Need to check at the time of Due Diligence)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -636,6 +645,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1098,11 +1122,11 @@
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
@@ -1136,7 +1160,7 @@
     </xf>
     <xf numFmtId="2" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="43" fontId="3" fillId="6" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1320,10 +1344,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1337,6 +1360,15 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="25" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1357,6 +1389,18 @@
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="43" fontId="3" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -1385,21 +1429,9 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1407,12 +1439,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1479,7 +1505,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1514,7 +1540,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1725,17 +1751,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="B63" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B67" sqref="B67"/>
       <selection pane="topRight" activeCell="B67" sqref="B67"/>
       <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="D78" sqref="D78:E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.85546875" style="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="59" style="19" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="5" width="17.7109375" style="19" customWidth="1" collapsed="1"/>
     <col min="6" max="7" width="7.5703125" style="19" hidden="1" customWidth="1" collapsed="1"/>
     <col min="8" max="10" width="9.140625" style="19" hidden="1" customWidth="1" collapsed="1"/>
@@ -1746,13 +1772,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="102" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="102"/>
       <c r="F1" s="18" t="s">
         <v>45</v>
       </c>
@@ -1770,36 +1796,36 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="103" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
       <c r="F2" s="19" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="100" t="s">
+      <c r="A3" s="104" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="100"/>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
+      <c r="B3" s="104"/>
+      <c r="C3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="104"/>
     </row>
     <row r="4" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="101" t="s">
+      <c r="A4" s="105" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="102"/>
-      <c r="C4" s="102"/>
-      <c r="D4" s="119" t="s">
+      <c r="B4" s="106"/>
+      <c r="C4" s="106"/>
+      <c r="D4" s="97" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="120" t="s">
+      <c r="E4" s="98" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2619,8 +2645,8 @@
       <c r="E75" s="8"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="24" t="s">
-        <v>2</v>
+      <c r="A76" s="99" t="s">
+        <v>168</v>
       </c>
       <c r="B76" s="11"/>
       <c r="C76" s="11"/>
@@ -2642,19 +2668,19 @@
         <v>15. Net Profit/loss [13-14]</v>
       </c>
       <c r="B78" s="38">
-        <f>B73-B75-B77</f>
+        <f>B73-B75+B76-B77</f>
         <v>0</v>
       </c>
       <c r="C78" s="38">
-        <f>IF(B78="","",SUM((ROUND(C73-(C77+C75),2))))</f>
+        <f>IF(B78="","",SUM((ROUND((C73+C76)-(C77+C75),2))))</f>
         <v>0</v>
       </c>
       <c r="D78" s="38">
-        <f>IF(A78="","",SUM((ROUND(D73-(D77+D75),2))))</f>
+        <f t="shared" ref="D78:E78" si="17">IF(C78="","",SUM((ROUND((D73+D76)-(D77+D75),2))))</f>
         <v>0</v>
       </c>
       <c r="E78" s="38">
-        <f>IF(A78="","",SUM((ROUND(E73-(E77+E75),2))))</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -2717,19 +2743,19 @@
         <v>108</v>
       </c>
       <c r="B84" s="38">
-        <f t="shared" ref="B84:E84" si="17">B78-B80</f>
+        <f t="shared" ref="B84:E84" si="18">B78-B80</f>
         <v>0</v>
       </c>
       <c r="C84" s="38">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="D84" s="38">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="E84" s="38">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
@@ -2745,24 +2771,23 @@
         <v>109</v>
       </c>
       <c r="B86" s="39">
-        <f t="shared" ref="B86:E86" si="18">IFERROR((B84/B78),0)</f>
+        <f t="shared" ref="B86:E86" si="19">IFERROR((B84/B78),0)</f>
         <v>0</v>
       </c>
       <c r="C86" s="39">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="D86" s="39">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="E86" s="39">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="CF53" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="4">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
@@ -2785,29 +2810,29 @@
   <dimension ref="A1:M87"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="7" topLeftCell="B68" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B67" sqref="B67"/>
       <selection pane="topRight" activeCell="B67" sqref="B67"/>
       <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.7109375" style="45" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="63.85546875" style="45" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="5" width="17.7109375" style="45" customWidth="1" collapsed="1"/>
     <col min="6" max="13" width="17.7109375" style="45" hidden="1" customWidth="1" collapsed="1"/>
     <col min="14" max="16384" width="9.140625" style="45" hidden="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="115" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="107"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
       <c r="F1" s="40"/>
       <c r="G1" s="41"/>
       <c r="H1" s="41"/>
@@ -2828,13 +2853,13 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="108" t="s">
+      <c r="A2" s="116" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
+      <c r="B2" s="116"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
       <c r="F2" s="44"/>
       <c r="G2" s="44"/>
       <c r="H2" s="44"/>
@@ -2845,13 +2870,13 @@
       <c r="M2" s="44"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="110" t="s">
+      <c r="A3" s="118" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="110"/>
-      <c r="C3" s="110"/>
-      <c r="D3" s="110"/>
-      <c r="E3" s="110"/>
+      <c r="B3" s="118"/>
+      <c r="C3" s="118"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
       <c r="F3" s="46"/>
       <c r="G3" s="46"/>
       <c r="H3" s="46"/>
@@ -2862,15 +2887,15 @@
       <c r="M3" s="46"/>
     </row>
     <row r="4" spans="1:13" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="109" t="s">
+      <c r="A4" s="117" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="109"/>
-      <c r="C4" s="109"/>
-      <c r="D4" s="119" t="s">
+      <c r="B4" s="117"/>
+      <c r="C4" s="117"/>
+      <c r="D4" s="97" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="120" t="s">
+      <c r="E4" s="98" t="s">
         <v>39</v>
       </c>
       <c r="F4" s="47"/>
@@ -2889,7 +2914,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="105" t="s">
+      <c r="A5" s="113" t="s">
         <v>71</v>
       </c>
       <c r="B5" s="28">
@@ -2936,76 +2961,76 @@
         <f>'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="M5" s="91" t="e">
+      <c r="M5" s="90" t="e">
         <f>'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="106"/>
-      <c r="B6" s="111" t="str">
+      <c r="A6" s="114"/>
+      <c r="B6" s="109" t="str">
         <f>+'Operating Stmt.'!B6:B6</f>
         <v>Audited</v>
       </c>
-      <c r="C6" s="111" t="str">
+      <c r="C6" s="109" t="str">
         <f>+'Operating Stmt.'!C6:C6</f>
         <v>Audited</v>
       </c>
-      <c r="D6" s="111" t="str">
+      <c r="D6" s="109" t="str">
         <f>+'Operating Stmt.'!D6:D6</f>
         <v>Audited</v>
       </c>
-      <c r="E6" s="111" t="str">
+      <c r="E6" s="109" t="str">
         <f>+'Operating Stmt.'!E6:E6</f>
         <v>Estimated</v>
       </c>
-      <c r="F6" s="111" t="e">
+      <c r="F6" s="109" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="G6" s="111" t="e">
+      <c r="G6" s="109" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="H6" s="111" t="e">
+      <c r="H6" s="109" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="I6" s="111" t="e">
+      <c r="I6" s="109" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="J6" s="111" t="e">
+      <c r="J6" s="109" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="111" t="e">
+      <c r="K6" s="109" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="L6" s="111" t="e">
+      <c r="L6" s="109" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="M6" s="113" t="e">
+      <c r="M6" s="107" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="106"/>
-      <c r="B7" s="112"/>
-      <c r="C7" s="112"/>
-      <c r="D7" s="112"/>
-      <c r="E7" s="112"/>
-      <c r="F7" s="115"/>
-      <c r="G7" s="115"/>
-      <c r="H7" s="115"/>
-      <c r="I7" s="115"/>
-      <c r="J7" s="115"/>
-      <c r="K7" s="115"/>
-      <c r="L7" s="115"/>
-      <c r="M7" s="114"/>
+      <c r="A7" s="114"/>
+      <c r="B7" s="119"/>
+      <c r="C7" s="119"/>
+      <c r="D7" s="119"/>
+      <c r="E7" s="119"/>
+      <c r="F7" s="110"/>
+      <c r="G7" s="110"/>
+      <c r="H7" s="110"/>
+      <c r="I7" s="110"/>
+      <c r="J7" s="110"/>
+      <c r="K7" s="110"/>
+      <c r="L7" s="110"/>
+      <c r="M7" s="108"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="53" t="s">
@@ -3024,7 +3049,7 @@
       <c r="L8" s="49"/>
       <c r="M8" s="50"/>
     </row>
-    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>69</v>
       </c>
@@ -3174,7 +3199,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M15" s="92">
+      <c r="M15" s="91">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3258,7 +3283,7 @@
       <c r="L20" s="2"/>
       <c r="M20" s="3"/>
     </row>
-    <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="26" t="s">
         <v>62</v>
       </c>
@@ -3354,7 +3379,7 @@
       <c r="L26" s="2"/>
       <c r="M26" s="3"/>
     </row>
-    <row r="27" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="26" t="s">
         <v>59</v>
       </c>
@@ -3386,7 +3411,7 @@
       <c r="L28" s="2"/>
       <c r="M28" s="3"/>
     </row>
-    <row r="29" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="58" t="s">
         <v>58</v>
       </c>
@@ -3433,7 +3458,7 @@
       <c r="L31" s="2"/>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="59" t="s">
         <v>57</v>
       </c>
@@ -3451,7 +3476,7 @@
       <c r="M32" s="3"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="103"/>
+      <c r="A33" s="111"/>
       <c r="B33" s="55"/>
       <c r="C33" s="55"/>
       <c r="D33" s="55"/>
@@ -3466,7 +3491,7 @@
       <c r="M33" s="3"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="104"/>
+      <c r="A34" s="112"/>
       <c r="B34" s="55"/>
       <c r="C34" s="55"/>
       <c r="D34" s="55"/>
@@ -3528,7 +3553,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M35" s="92">
+      <c r="M35" s="91">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3548,7 +3573,7 @@
       <c r="L36" s="2"/>
       <c r="M36" s="3"/>
     </row>
-    <row r="37" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="62" t="s">
         <v>55</v>
       </c>
@@ -3596,7 +3621,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M37" s="92">
+      <c r="M37" s="91">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3712,7 +3737,7 @@
       <c r="L44" s="2"/>
       <c r="M44" s="3"/>
     </row>
-    <row r="45" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="26" t="s">
         <v>52</v>
       </c>
@@ -3960,7 +3985,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="M55" s="92">
+      <c r="M55" s="91">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -3984,24 +4009,24 @@
       <c r="A57" s="67" t="s">
         <v>113</v>
       </c>
-      <c r="B57" s="56">
+      <c r="B57" s="100">
         <f>SUM(ROUND(B58+B59+B60+B61,2))</f>
         <v>0</v>
       </c>
-      <c r="C57" s="56">
-        <f t="shared" ref="C57:M57" si="5">SUM(ROUND(C58+C59+C60+C61,2))</f>
-        <v>0</v>
-      </c>
-      <c r="D57" s="56">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E57" s="56">
-        <f t="shared" si="5"/>
+      <c r="C57" s="100">
+        <f>SUM(ROUND(C58+C59+C60+C61,2))</f>
+        <v>0</v>
+      </c>
+      <c r="D57" s="100">
+        <f>SUM(ROUND(D58+D59+D60+D61,2))</f>
+        <v>0</v>
+      </c>
+      <c r="E57" s="100">
+        <f>SUM(ROUND(E58+E59+E60+E61,2))</f>
         <v>0</v>
       </c>
       <c r="F57" s="56">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="F57:M57" si="5">SUM(ROUND(F58+F59+F60+F61,2))</f>
         <v>0</v>
       </c>
       <c r="G57" s="56">
@@ -4102,7 +4127,6 @@
       <c r="M61" s="17"/>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A62" s="24"/>
       <c r="B62" s="55"/>
       <c r="C62" s="55"/>
       <c r="D62" s="55"/>
@@ -4116,28 +4140,28 @@
       <c r="L62" s="2"/>
       <c r="M62" s="3"/>
     </row>
-    <row r="63" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="B63" s="57">
-        <f t="shared" ref="B63:M63" si="6">SUM(ROUND(B37+B55+B57,2))</f>
-        <v>0</v>
-      </c>
-      <c r="C63" s="57">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="D63" s="57">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="E63" s="57">
-        <f t="shared" si="6"/>
+      <c r="B63" s="101">
+        <f>SUM(ROUND(B37+B55+B57,2))</f>
+        <v>0</v>
+      </c>
+      <c r="C63" s="101">
+        <f>SUM(ROUND(C37+C55+C57,2))</f>
+        <v>0</v>
+      </c>
+      <c r="D63" s="101">
+        <f>SUM(ROUND(D37+D55+D57,2))</f>
+        <v>0</v>
+      </c>
+      <c r="E63" s="101">
+        <f>SUM(ROUND(E37+E55+E57,2))</f>
         <v>0</v>
       </c>
       <c r="F63" s="57">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="F63:M63" si="6">SUM(ROUND(F37+F55+F57,2))</f>
         <v>0</v>
       </c>
       <c r="G63" s="57">
@@ -4164,7 +4188,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M63" s="92">
+      <c r="M63" s="91">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -4552,13 +4576,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="M85" s="92">
+      <c r="M85" s="91">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A86" s="24"/>
+      <c r="A86" s="99" t="s">
+        <v>169</v>
+      </c>
       <c r="B86" s="55"/>
       <c r="C86" s="55"/>
       <c r="D86" s="55"/>
@@ -4577,23 +4603,23 @@
         <v>124</v>
       </c>
       <c r="B87" s="71">
-        <f>SUM(ROUND(B63+B85,2))</f>
+        <f>SUM(ROUND(B63+B85+B86,2))</f>
         <v>0</v>
       </c>
       <c r="C87" s="71">
-        <f t="shared" ref="C87:M87" si="8">SUM(ROUND(C63+C85,2))</f>
+        <f>SUM(ROUND(C63+C85+C86,2))</f>
         <v>0</v>
       </c>
       <c r="D87" s="71">
-        <f t="shared" si="8"/>
+        <f>SUM(ROUND(D63+D85+D86,2))</f>
         <v>0</v>
       </c>
       <c r="E87" s="71">
-        <f t="shared" si="8"/>
+        <f>SUM(ROUND(E63+E85+E86,2))</f>
         <v>0</v>
       </c>
       <c r="F87" s="71">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="F87:M87" si="8">SUM(ROUND(F63+F85,2))</f>
         <v>0</v>
       </c>
       <c r="G87" s="71">
@@ -4620,7 +4646,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="M87" s="93">
+      <c r="M87" s="92">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -4628,14 +4654,6 @@
   </sheetData>
   <sheetProtection password="CF53" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="18">
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="H6:H7"/>
     <mergeCell ref="A33:A34"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="A1:E1"/>
@@ -4646,6 +4664,14 @@
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="H6:H7"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:M13 B17:M32 B82:M83 B41:M53 B67:M80 B57:M57">
@@ -4664,30 +4690,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M99"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="7" topLeftCell="B82" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B67" sqref="B67"/>
       <selection pane="topRight" activeCell="B67" sqref="B67"/>
       <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="A89" sqref="A89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.140625" style="74" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="63.85546875" style="74" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="5" width="17.7109375" style="45" customWidth="1" collapsed="1"/>
     <col min="6" max="13" width="17.7109375" style="45" hidden="1" customWidth="1" collapsed="1"/>
     <col min="14" max="16384" width="0" style="45" hidden="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="115" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="107"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
       <c r="F1" s="41"/>
       <c r="G1" s="41"/>
       <c r="H1" s="41"/>
@@ -4708,13 +4734,13 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="108" t="s">
+      <c r="A2" s="116" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
+      <c r="B2" s="116"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
       <c r="F2" s="44"/>
       <c r="G2" s="44"/>
       <c r="H2" s="44"/>
@@ -4725,13 +4751,13 @@
       <c r="M2" s="44"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="110" t="s">
+      <c r="A3" s="118" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="110"/>
-      <c r="C3" s="110"/>
-      <c r="D3" s="110"/>
-      <c r="E3" s="110"/>
+      <c r="B3" s="118"/>
+      <c r="C3" s="118"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
       <c r="F3" s="46"/>
       <c r="G3" s="46"/>
       <c r="H3" s="46"/>
@@ -4742,15 +4768,15 @@
       <c r="M3" s="46"/>
     </row>
     <row r="4" spans="1:13" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="109" t="s">
+      <c r="A4" s="117" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="109"/>
-      <c r="C4" s="109"/>
-      <c r="D4" s="119" t="s">
+      <c r="B4" s="117"/>
+      <c r="C4" s="117"/>
+      <c r="D4" s="97" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="120" t="s">
+      <c r="E4" s="98" t="s">
         <v>39</v>
       </c>
       <c r="F4" s="47"/>
@@ -4769,7 +4795,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="117" t="s">
+      <c r="A5" s="121" t="s">
         <v>95</v>
       </c>
       <c r="B5" s="75">
@@ -4816,76 +4842,76 @@
         <f>'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="M5" s="94" t="e">
+      <c r="M5" s="93" t="e">
         <f>'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="118"/>
-      <c r="B6" s="111" t="str">
+      <c r="A6" s="122"/>
+      <c r="B6" s="109" t="str">
         <f>Liabilities!B6</f>
         <v>Audited</v>
       </c>
-      <c r="C6" s="111" t="str">
+      <c r="C6" s="109" t="str">
         <f>Liabilities!C6</f>
         <v>Audited</v>
       </c>
-      <c r="D6" s="111" t="str">
+      <c r="D6" s="109" t="str">
         <f>Liabilities!D6</f>
         <v>Audited</v>
       </c>
-      <c r="E6" s="111" t="str">
+      <c r="E6" s="109" t="str">
         <f>Liabilities!E6</f>
         <v>Estimated</v>
       </c>
-      <c r="F6" s="111" t="e">
+      <c r="F6" s="109" t="e">
         <f>Liabilities!F6</f>
         <v>#REF!</v>
       </c>
-      <c r="G6" s="111" t="e">
+      <c r="G6" s="109" t="e">
         <f>Liabilities!G6</f>
         <v>#REF!</v>
       </c>
-      <c r="H6" s="111" t="e">
+      <c r="H6" s="109" t="e">
         <f>Liabilities!H6</f>
         <v>#REF!</v>
       </c>
-      <c r="I6" s="111" t="e">
+      <c r="I6" s="109" t="e">
         <f>Liabilities!I6</f>
         <v>#REF!</v>
       </c>
-      <c r="J6" s="111" t="e">
+      <c r="J6" s="109" t="e">
         <f>Liabilities!J6</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="111" t="e">
+      <c r="K6" s="109" t="e">
         <f>Liabilities!K6</f>
         <v>#REF!</v>
       </c>
-      <c r="L6" s="111" t="e">
+      <c r="L6" s="109" t="e">
         <f>Liabilities!L6</f>
         <v>#REF!</v>
       </c>
-      <c r="M6" s="113" t="e">
+      <c r="M6" s="107" t="e">
         <f>Liabilities!M6</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="118"/>
-      <c r="B7" s="112"/>
-      <c r="C7" s="112"/>
-      <c r="D7" s="112"/>
-      <c r="E7" s="112"/>
-      <c r="F7" s="112"/>
-      <c r="G7" s="112"/>
-      <c r="H7" s="112"/>
-      <c r="I7" s="112"/>
-      <c r="J7" s="112"/>
-      <c r="K7" s="112"/>
-      <c r="L7" s="112"/>
-      <c r="M7" s="116"/>
+      <c r="A7" s="122"/>
+      <c r="B7" s="119"/>
+      <c r="C7" s="119"/>
+      <c r="D7" s="119"/>
+      <c r="E7" s="119"/>
+      <c r="F7" s="119"/>
+      <c r="G7" s="119"/>
+      <c r="H7" s="119"/>
+      <c r="I7" s="119"/>
+      <c r="J7" s="119"/>
+      <c r="K7" s="119"/>
+      <c r="L7" s="119"/>
+      <c r="M7" s="120"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="76" t="s">
@@ -4936,7 +4962,7 @@
       <c r="L10" s="2"/>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="81" t="s">
         <v>167</v>
       </c>
@@ -4984,7 +5010,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M11" s="95">
+      <c r="M11" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5057,7 +5083,7 @@
       <c r="L15" s="2"/>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="81" t="s">
         <v>129</v>
       </c>
@@ -5125,7 +5151,7 @@
       <c r="L19" s="2"/>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="81" t="s">
         <v>130</v>
       </c>
@@ -5205,7 +5231,7 @@
         <f t="shared" si="1"/>
         <v>#REF!</v>
       </c>
-      <c r="M22" s="95" t="e">
+      <c r="M22" s="94" t="e">
         <f t="shared" si="1"/>
         <v>#REF!</v>
       </c>
@@ -5273,7 +5299,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M24" s="92">
+      <c r="M24" s="91">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -5348,22 +5374,10 @@
       <c r="A29" s="79" t="s">
         <v>88</v>
       </c>
-      <c r="B29" s="82">
-        <f>'Operating Stmt.'!B42</f>
-        <v>0</v>
-      </c>
-      <c r="C29" s="82">
-        <f>'Operating Stmt.'!C42</f>
-        <v>0</v>
-      </c>
-      <c r="D29" s="82">
-        <f>'Operating Stmt.'!D42</f>
-        <v>0</v>
-      </c>
-      <c r="E29" s="82">
-        <f>'Operating Stmt.'!E42</f>
-        <v>0</v>
-      </c>
+      <c r="B29" s="82"/>
+      <c r="C29" s="82"/>
+      <c r="D29" s="82"/>
+      <c r="E29" s="82"/>
       <c r="F29" s="82" t="e">
         <f>'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
@@ -5392,7 +5406,7 @@
         <f>'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="M29" s="95" t="e">
+      <c r="M29" s="94" t="e">
         <f>'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
@@ -5416,22 +5430,10 @@
       <c r="A31" s="79" t="s">
         <v>87</v>
       </c>
-      <c r="B31" s="82">
-        <f>'Operating Stmt.'!B50</f>
-        <v>0</v>
-      </c>
-      <c r="C31" s="82">
-        <f>'Operating Stmt.'!C50</f>
-        <v>0</v>
-      </c>
-      <c r="D31" s="82">
-        <f>'Operating Stmt.'!D50</f>
-        <v>0</v>
-      </c>
-      <c r="E31" s="82">
-        <f>'Operating Stmt.'!E50</f>
-        <v>0</v>
-      </c>
+      <c r="B31" s="82"/>
+      <c r="C31" s="82"/>
+      <c r="D31" s="82"/>
+      <c r="E31" s="82"/>
       <c r="F31" s="82" t="e">
         <f>'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
@@ -5460,7 +5462,7 @@
         <f>'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="M31" s="95" t="e">
+      <c r="M31" s="94" t="e">
         <f>'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
@@ -5528,7 +5530,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M33" s="92">
+      <c r="M33" s="91">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -5582,7 +5584,7 @@
       <c r="L36" s="2"/>
       <c r="M36" s="3"/>
     </row>
-    <row r="37" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="81" t="s">
         <v>132</v>
       </c>
@@ -5648,7 +5650,7 @@
       <c r="L40" s="2"/>
       <c r="M40" s="3"/>
     </row>
-    <row r="41" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="81" t="s">
         <v>134</v>
       </c>
@@ -5728,7 +5730,7 @@
         <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
-      <c r="M43" s="92" t="e">
+      <c r="M43" s="91" t="e">
         <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
@@ -5748,7 +5750,7 @@
       <c r="L44" s="2"/>
       <c r="M44" s="3"/>
     </row>
-    <row r="45" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="81" t="s">
         <v>136</v>
       </c>
@@ -6141,7 +6143,7 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="M62" s="92">
+      <c r="M62" s="91">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -6212,7 +6214,7 @@
       <c r="L66" s="2"/>
       <c r="M66" s="3"/>
     </row>
-    <row r="67" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="81" t="s">
         <v>79</v>
       </c>
@@ -6246,7 +6248,7 @@
       <c r="L68" s="2"/>
       <c r="M68" s="3"/>
     </row>
-    <row r="69" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="81" t="s">
         <v>77</v>
       </c>
@@ -6328,7 +6330,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="M71" s="96">
+      <c r="M71" s="95">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -6433,7 +6435,7 @@
       <c r="L77" s="2"/>
       <c r="M77" s="3"/>
     </row>
-    <row r="78" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="81" t="s">
         <v>148</v>
       </c>
@@ -6533,7 +6535,7 @@
       <c r="L81" s="2"/>
       <c r="M81" s="3"/>
     </row>
-    <row r="82" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="81" t="s">
         <v>150</v>
       </c>
@@ -6581,7 +6583,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M82" s="95">
+      <c r="M82" s="94">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -6672,7 +6674,9 @@
       <c r="M87" s="3"/>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A88" s="88"/>
+      <c r="A88" s="99" t="s">
+        <v>170</v>
+      </c>
       <c r="B88" s="80"/>
       <c r="C88" s="80"/>
       <c r="D88" s="80"/>
@@ -6691,23 +6695,23 @@
         <v>154</v>
       </c>
       <c r="B89" s="82">
-        <f>SUM(ROUND(B43+B56+B80+B82,2))</f>
+        <f>SUM(ROUND(B43+B56+B80+B82+B88,2))</f>
         <v>0</v>
       </c>
       <c r="C89" s="82">
-        <f t="shared" ref="C89:M89" si="11">SUM(ROUND(C43+C56+C80+C82,2))</f>
+        <f>SUM(ROUND(C43+C56+C80+C82+C88,2))</f>
         <v>0</v>
       </c>
       <c r="D89" s="82">
-        <f t="shared" si="11"/>
+        <f>SUM(ROUND(D43+D56+D80+D82+D88,2))</f>
         <v>0</v>
       </c>
       <c r="E89" s="82">
-        <f t="shared" si="11"/>
+        <f>SUM(ROUND(E43+E56+E80+E82+E88,2))</f>
         <v>0</v>
       </c>
       <c r="F89" s="82" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="F89:M89" si="11">SUM(ROUND(F43+F56+F80+F82,2))</f>
         <v>#REF!</v>
       </c>
       <c r="G89" s="82" t="e">
@@ -6802,7 +6806,7 @@
         <f>ROUND(Liabilities!L85-Liabilities!L75-Asset!L82,2)</f>
         <v>0</v>
       </c>
-      <c r="M91" s="95">
+      <c r="M91" s="94">
         <f>ROUND(Liabilities!M85-Liabilities!M75-Asset!M82,2)</f>
         <v>0</v>
       </c>
@@ -6870,7 +6874,7 @@
         <f>SUM(ROUND(Liabilities!L55+Liabilities!L85,2))-(ROUND(L56+L80+L82,2))</f>
         <v>0</v>
       </c>
-      <c r="M93" s="95">
+      <c r="M93" s="94">
         <f>SUM(ROUND(Liabilities!M55+Liabilities!M85,2))-(ROUND(M56+M80+M82,2))</f>
         <v>0</v>
       </c>
@@ -6938,7 +6942,7 @@
         <f>IF(Liabilities!L37=0,0,(ROUND(L43/Liabilities!L37,2)))</f>
         <v>0</v>
       </c>
-      <c r="M95" s="95">
+      <c r="M95" s="94">
         <f>IF(Liabilities!M37=0,0,(ROUND(M43/Liabilities!M37,2)))</f>
         <v>0</v>
       </c>
@@ -7006,7 +7010,7 @@
         <f>IF(L91=0,0,(ROUND(Liabilities!L63/L91,2)))</f>
         <v>0</v>
       </c>
-      <c r="M97" s="95">
+      <c r="M97" s="94">
         <f>IF(M91=0,0,(ROUND(Liabilities!M63/M91,2)))</f>
         <v>0</v>
       </c>
@@ -7027,60 +7031,59 @@
       <c r="M98" s="3"/>
     </row>
     <row r="99" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="89" t="s">
+      <c r="A99" s="88" t="s">
         <v>153</v>
       </c>
-      <c r="B99" s="90">
+      <c r="B99" s="89">
         <f>IF(B91=0,0,(ROUND(Liabilities!B55/B91,2)))</f>
         <v>0</v>
       </c>
-      <c r="C99" s="90">
+      <c r="C99" s="89">
         <f>IF(C91=0,0,(ROUND(Liabilities!C55/C91,2)))</f>
         <v>0</v>
       </c>
-      <c r="D99" s="90">
+      <c r="D99" s="89">
         <f>IF(D91=0,0,(ROUND(Liabilities!D55/D91,2)))</f>
         <v>0</v>
       </c>
-      <c r="E99" s="90">
+      <c r="E99" s="89">
         <f>IF(E91=0,0,(ROUND(Liabilities!E55/E91,2)))</f>
         <v>0</v>
       </c>
-      <c r="F99" s="90">
+      <c r="F99" s="89">
         <f>IF(F91=0,0,(ROUND(Liabilities!F55/F91,2)))</f>
         <v>0</v>
       </c>
-      <c r="G99" s="90">
+      <c r="G99" s="89">
         <f>IF(G91=0,0,(ROUND(Liabilities!G55/G91,2)))</f>
         <v>0</v>
       </c>
-      <c r="H99" s="90">
+      <c r="H99" s="89">
         <f>IF(H91=0,0,(ROUND(Liabilities!H55/H91,2)))</f>
         <v>0</v>
       </c>
-      <c r="I99" s="90">
+      <c r="I99" s="89">
         <f>IF(I91=0,0,(ROUND(Liabilities!I55/I91,2)))</f>
         <v>0</v>
       </c>
-      <c r="J99" s="90">
+      <c r="J99" s="89">
         <f>IF(J91=0,0,(ROUND(Liabilities!J55/J91,2)))</f>
         <v>0</v>
       </c>
-      <c r="K99" s="90">
+      <c r="K99" s="89">
         <f>IF(K91=0,0,(ROUND(Liabilities!K55/K91,2)))</f>
         <v>0</v>
       </c>
-      <c r="L99" s="90">
+      <c r="L99" s="89">
         <f>IF(L91=0,0,(ROUND(Liabilities!L55/L91,2)))</f>
         <v>0</v>
       </c>
-      <c r="M99" s="97">
+      <c r="M99" s="96">
         <f>IF(M91=0,0,(ROUND(Liabilities!M55/M91,2)))</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="CF53" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="17">
     <mergeCell ref="M6:M7"/>
     <mergeCell ref="A5:A7"/>

</xml_diff>

<commit_message>
final cma template changes shruthi.
</commit_message>
<xml_diff>
--- a/service-loans/template/Template_CW_CMA.xlsx
+++ b/service-loans/template/Template_CW_CMA.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="nMIDBcyH02QIBA4bXtkulhW+BkwLjO6uUdnHuLe/vey9rIzKWc8NDkCsYZON8UKSky/yikEzYHsiuF6pBe7KDg==" workbookSaltValue="OCFZwCBGKUImSpaXHpKcuQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Operating Stmt." sheetId="2" r:id="rId1"/>
     <sheet name="Liabilities" sheetId="3" r:id="rId2"/>
     <sheet name="Asset" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -560,8 +560,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -1122,9 +1122,9 @@
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1160,7 +1160,7 @@
     </xf>
     <xf numFmtId="2" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="43" fontId="3" fillId="6" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1344,7 +1344,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -1389,18 +1389,6 @@
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -1429,7 +1417,19 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1505,7 +1505,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1540,7 +1540,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1751,12 +1751,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R86"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B63" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B67" sqref="B67"/>
       <selection pane="topRight" activeCell="B67" sqref="B67"/>
       <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
-      <selection pane="bottomRight" activeCell="D78" sqref="D78:E78"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -2660,7 +2660,7 @@
       <c r="B77" s="11"/>
       <c r="C77" s="11"/>
       <c r="D77" s="11"/>
-      <c r="E77" s="8"/>
+      <c r="E77" s="11"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="24" t="str">
@@ -2788,6 +2788,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection password="CF53" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="4">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
@@ -2810,11 +2811,11 @@
   <dimension ref="A1:M87"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="B68" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B67" sqref="B67"/>
       <selection pane="topRight" activeCell="B67" sqref="B67"/>
       <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
-      <selection pane="bottomRight" activeCell="E87" sqref="E87"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -2826,13 +2827,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="111" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
+      <c r="B1" s="111"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
       <c r="F1" s="40"/>
       <c r="G1" s="41"/>
       <c r="H1" s="41"/>
@@ -2853,13 +2854,13 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="116" t="s">
+      <c r="A2" s="112" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="116"/>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
+      <c r="B2" s="112"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
       <c r="F2" s="44"/>
       <c r="G2" s="44"/>
       <c r="H2" s="44"/>
@@ -2870,13 +2871,13 @@
       <c r="M2" s="44"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="118" t="s">
+      <c r="A3" s="114" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="118"/>
-      <c r="C3" s="118"/>
-      <c r="D3" s="118"/>
-      <c r="E3" s="118"/>
+      <c r="B3" s="114"/>
+      <c r="C3" s="114"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="114"/>
       <c r="F3" s="46"/>
       <c r="G3" s="46"/>
       <c r="H3" s="46"/>
@@ -2887,11 +2888,11 @@
       <c r="M3" s="46"/>
     </row>
     <row r="4" spans="1:13" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="117" t="s">
+      <c r="A4" s="113" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="117"/>
-      <c r="C4" s="117"/>
+      <c r="B4" s="113"/>
+      <c r="C4" s="113"/>
       <c r="D4" s="97" t="s">
         <v>40</v>
       </c>
@@ -2914,7 +2915,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="113" t="s">
+      <c r="A5" s="109" t="s">
         <v>71</v>
       </c>
       <c r="B5" s="28">
@@ -2967,70 +2968,70 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="114"/>
-      <c r="B6" s="109" t="str">
+      <c r="A6" s="110"/>
+      <c r="B6" s="115" t="str">
         <f>+'Operating Stmt.'!B6:B6</f>
         <v>Audited</v>
       </c>
-      <c r="C6" s="109" t="str">
+      <c r="C6" s="115" t="str">
         <f>+'Operating Stmt.'!C6:C6</f>
         <v>Audited</v>
       </c>
-      <c r="D6" s="109" t="str">
+      <c r="D6" s="115" t="str">
         <f>+'Operating Stmt.'!D6:D6</f>
         <v>Audited</v>
       </c>
-      <c r="E6" s="109" t="str">
+      <c r="E6" s="115" t="str">
         <f>+'Operating Stmt.'!E6:E6</f>
         <v>Estimated</v>
       </c>
-      <c r="F6" s="109" t="e">
+      <c r="F6" s="115" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="G6" s="109" t="e">
+      <c r="G6" s="115" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="H6" s="109" t="e">
+      <c r="H6" s="115" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="I6" s="109" t="e">
+      <c r="I6" s="115" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="J6" s="109" t="e">
+      <c r="J6" s="115" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="109" t="e">
+      <c r="K6" s="115" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="L6" s="109" t="e">
+      <c r="L6" s="115" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="M6" s="107" t="e">
+      <c r="M6" s="117" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="114"/>
-      <c r="B7" s="119"/>
-      <c r="C7" s="119"/>
-      <c r="D7" s="119"/>
-      <c r="E7" s="119"/>
-      <c r="F7" s="110"/>
-      <c r="G7" s="110"/>
-      <c r="H7" s="110"/>
-      <c r="I7" s="110"/>
-      <c r="J7" s="110"/>
-      <c r="K7" s="110"/>
-      <c r="L7" s="110"/>
-      <c r="M7" s="108"/>
+      <c r="A7" s="110"/>
+      <c r="B7" s="116"/>
+      <c r="C7" s="116"/>
+      <c r="D7" s="116"/>
+      <c r="E7" s="116"/>
+      <c r="F7" s="119"/>
+      <c r="G7" s="119"/>
+      <c r="H7" s="119"/>
+      <c r="I7" s="119"/>
+      <c r="J7" s="119"/>
+      <c r="K7" s="119"/>
+      <c r="L7" s="119"/>
+      <c r="M7" s="118"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="53" t="s">
@@ -3476,7 +3477,7 @@
       <c r="M32" s="3"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="111"/>
+      <c r="A33" s="107"/>
       <c r="B33" s="55"/>
       <c r="C33" s="55"/>
       <c r="D33" s="55"/>
@@ -3491,7 +3492,7 @@
       <c r="M33" s="3"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="112"/>
+      <c r="A34" s="108"/>
       <c r="B34" s="55"/>
       <c r="C34" s="55"/>
       <c r="D34" s="55"/>
@@ -4588,7 +4589,7 @@
       <c r="B86" s="55"/>
       <c r="C86" s="55"/>
       <c r="D86" s="55"/>
-      <c r="E86" s="2"/>
+      <c r="E86" s="55"/>
       <c r="F86" s="2"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
@@ -4654,6 +4655,14 @@
   </sheetData>
   <sheetProtection password="CF53" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="18">
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="H6:H7"/>
     <mergeCell ref="A33:A34"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="A1:E1"/>
@@ -4664,14 +4673,6 @@
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="H6:H7"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:M13 B17:M32 B82:M83 B41:M53 B67:M80 B57:M57">
@@ -4690,12 +4691,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="B82" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B67" sqref="B67"/>
       <selection pane="topRight" activeCell="B67" sqref="B67"/>
       <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
-      <selection pane="bottomRight" activeCell="A89" sqref="A89"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -4707,13 +4708,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="111" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
+      <c r="B1" s="111"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
       <c r="F1" s="41"/>
       <c r="G1" s="41"/>
       <c r="H1" s="41"/>
@@ -4734,13 +4735,13 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="116" t="s">
+      <c r="A2" s="112" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="116"/>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
+      <c r="B2" s="112"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
       <c r="F2" s="44"/>
       <c r="G2" s="44"/>
       <c r="H2" s="44"/>
@@ -4751,13 +4752,13 @@
       <c r="M2" s="44"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="118" t="s">
+      <c r="A3" s="114" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="118"/>
-      <c r="C3" s="118"/>
-      <c r="D3" s="118"/>
-      <c r="E3" s="118"/>
+      <c r="B3" s="114"/>
+      <c r="C3" s="114"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="114"/>
       <c r="F3" s="46"/>
       <c r="G3" s="46"/>
       <c r="H3" s="46"/>
@@ -4768,11 +4769,11 @@
       <c r="M3" s="46"/>
     </row>
     <row r="4" spans="1:13" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="117" t="s">
+      <c r="A4" s="113" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="117"/>
-      <c r="C4" s="117"/>
+      <c r="B4" s="113"/>
+      <c r="C4" s="113"/>
       <c r="D4" s="97" t="s">
         <v>40</v>
       </c>
@@ -4849,68 +4850,68 @@
     </row>
     <row r="6" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="122"/>
-      <c r="B6" s="109" t="str">
+      <c r="B6" s="115" t="str">
         <f>Liabilities!B6</f>
         <v>Audited</v>
       </c>
-      <c r="C6" s="109" t="str">
+      <c r="C6" s="115" t="str">
         <f>Liabilities!C6</f>
         <v>Audited</v>
       </c>
-      <c r="D6" s="109" t="str">
+      <c r="D6" s="115" t="str">
         <f>Liabilities!D6</f>
         <v>Audited</v>
       </c>
-      <c r="E6" s="109" t="str">
+      <c r="E6" s="115" t="str">
         <f>Liabilities!E6</f>
         <v>Estimated</v>
       </c>
-      <c r="F6" s="109" t="e">
+      <c r="F6" s="115" t="e">
         <f>Liabilities!F6</f>
         <v>#REF!</v>
       </c>
-      <c r="G6" s="109" t="e">
+      <c r="G6" s="115" t="e">
         <f>Liabilities!G6</f>
         <v>#REF!</v>
       </c>
-      <c r="H6" s="109" t="e">
+      <c r="H6" s="115" t="e">
         <f>Liabilities!H6</f>
         <v>#REF!</v>
       </c>
-      <c r="I6" s="109" t="e">
+      <c r="I6" s="115" t="e">
         <f>Liabilities!I6</f>
         <v>#REF!</v>
       </c>
-      <c r="J6" s="109" t="e">
+      <c r="J6" s="115" t="e">
         <f>Liabilities!J6</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="109" t="e">
+      <c r="K6" s="115" t="e">
         <f>Liabilities!K6</f>
         <v>#REF!</v>
       </c>
-      <c r="L6" s="109" t="e">
+      <c r="L6" s="115" t="e">
         <f>Liabilities!L6</f>
         <v>#REF!</v>
       </c>
-      <c r="M6" s="107" t="e">
+      <c r="M6" s="117" t="e">
         <f>Liabilities!M6</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="122"/>
-      <c r="B7" s="119"/>
-      <c r="C7" s="119"/>
-      <c r="D7" s="119"/>
-      <c r="E7" s="119"/>
-      <c r="F7" s="119"/>
-      <c r="G7" s="119"/>
-      <c r="H7" s="119"/>
-      <c r="I7" s="119"/>
-      <c r="J7" s="119"/>
-      <c r="K7" s="119"/>
-      <c r="L7" s="119"/>
+      <c r="B7" s="116"/>
+      <c r="C7" s="116"/>
+      <c r="D7" s="116"/>
+      <c r="E7" s="116"/>
+      <c r="F7" s="116"/>
+      <c r="G7" s="116"/>
+      <c r="H7" s="116"/>
+      <c r="I7" s="116"/>
+      <c r="J7" s="116"/>
+      <c r="K7" s="116"/>
+      <c r="L7" s="116"/>
       <c r="M7" s="120"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -6680,7 +6681,7 @@
       <c r="B88" s="80"/>
       <c r="C88" s="80"/>
       <c r="D88" s="80"/>
-      <c r="E88" s="5"/>
+      <c r="E88" s="80"/>
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
@@ -7084,7 +7085,12 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection password="CF53" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="17">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:C4"/>
     <mergeCell ref="M6:M7"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="B6:B7"/>
@@ -7098,10 +7104,6 @@
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="K6:K7"/>
     <mergeCell ref="L6:L7"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="50" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
new template added Template_CW_CMA.xlsx
</commit_message>
<xml_diff>
--- a/service-loans/template/Template_CW_CMA.xlsx
+++ b/service-loans/template/Template_CW_CMA.xlsx
@@ -1389,6 +1389,18 @@
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -1417,19 +1429,7 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2827,13 +2827,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="115" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="111"/>
-      <c r="C1" s="111"/>
-      <c r="D1" s="111"/>
-      <c r="E1" s="111"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
       <c r="F1" s="40"/>
       <c r="G1" s="41"/>
       <c r="H1" s="41"/>
@@ -2854,13 +2854,13 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="112" t="s">
+      <c r="A2" s="116" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="112"/>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
+      <c r="B2" s="116"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
       <c r="F2" s="44"/>
       <c r="G2" s="44"/>
       <c r="H2" s="44"/>
@@ -2871,13 +2871,13 @@
       <c r="M2" s="44"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="114" t="s">
+      <c r="A3" s="118" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="114"/>
-      <c r="C3" s="114"/>
-      <c r="D3" s="114"/>
-      <c r="E3" s="114"/>
+      <c r="B3" s="118"/>
+      <c r="C3" s="118"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
       <c r="F3" s="46"/>
       <c r="G3" s="46"/>
       <c r="H3" s="46"/>
@@ -2888,11 +2888,11 @@
       <c r="M3" s="46"/>
     </row>
     <row r="4" spans="1:13" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="113" t="s">
+      <c r="A4" s="117" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="113"/>
-      <c r="C4" s="113"/>
+      <c r="B4" s="117"/>
+      <c r="C4" s="117"/>
       <c r="D4" s="97" t="s">
         <v>40</v>
       </c>
@@ -2915,7 +2915,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="109" t="s">
+      <c r="A5" s="113" t="s">
         <v>71</v>
       </c>
       <c r="B5" s="28">
@@ -2968,70 +2968,70 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="110"/>
-      <c r="B6" s="115" t="str">
+      <c r="A6" s="114"/>
+      <c r="B6" s="109" t="str">
         <f>+'Operating Stmt.'!B6:B6</f>
         <v>Audited</v>
       </c>
-      <c r="C6" s="115" t="str">
+      <c r="C6" s="109" t="str">
         <f>+'Operating Stmt.'!C6:C6</f>
         <v>Audited</v>
       </c>
-      <c r="D6" s="115" t="str">
+      <c r="D6" s="109" t="str">
         <f>+'Operating Stmt.'!D6:D6</f>
         <v>Audited</v>
       </c>
-      <c r="E6" s="115" t="str">
+      <c r="E6" s="109" t="str">
         <f>+'Operating Stmt.'!E6:E6</f>
         <v>Estimated</v>
       </c>
-      <c r="F6" s="115" t="e">
+      <c r="F6" s="109" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="G6" s="115" t="e">
+      <c r="G6" s="109" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="H6" s="115" t="e">
+      <c r="H6" s="109" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="I6" s="115" t="e">
+      <c r="I6" s="109" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="J6" s="115" t="e">
+      <c r="J6" s="109" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="115" t="e">
+      <c r="K6" s="109" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="L6" s="115" t="e">
+      <c r="L6" s="109" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="M6" s="117" t="e">
+      <c r="M6" s="107" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="110"/>
-      <c r="B7" s="116"/>
-      <c r="C7" s="116"/>
-      <c r="D7" s="116"/>
-      <c r="E7" s="116"/>
-      <c r="F7" s="119"/>
-      <c r="G7" s="119"/>
-      <c r="H7" s="119"/>
-      <c r="I7" s="119"/>
-      <c r="J7" s="119"/>
-      <c r="K7" s="119"/>
-      <c r="L7" s="119"/>
-      <c r="M7" s="118"/>
+      <c r="A7" s="114"/>
+      <c r="B7" s="119"/>
+      <c r="C7" s="119"/>
+      <c r="D7" s="119"/>
+      <c r="E7" s="119"/>
+      <c r="F7" s="110"/>
+      <c r="G7" s="110"/>
+      <c r="H7" s="110"/>
+      <c r="I7" s="110"/>
+      <c r="J7" s="110"/>
+      <c r="K7" s="110"/>
+      <c r="L7" s="110"/>
+      <c r="M7" s="108"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="53" t="s">
@@ -3477,7 +3477,7 @@
       <c r="M32" s="3"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="107"/>
+      <c r="A33" s="111"/>
       <c r="B33" s="55"/>
       <c r="C33" s="55"/>
       <c r="D33" s="55"/>
@@ -3492,7 +3492,7 @@
       <c r="M33" s="3"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="108"/>
+      <c r="A34" s="112"/>
       <c r="B34" s="55"/>
       <c r="C34" s="55"/>
       <c r="D34" s="55"/>
@@ -4655,14 +4655,6 @@
   </sheetData>
   <sheetProtection password="CF53" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="18">
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="H6:H7"/>
     <mergeCell ref="A33:A34"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="A1:E1"/>
@@ -4673,6 +4665,14 @@
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="H6:H7"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:M13 B17:M32 B82:M83 B41:M53 B67:M80 B57:M57">
@@ -4708,13 +4708,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="115" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="111"/>
-      <c r="C1" s="111"/>
-      <c r="D1" s="111"/>
-      <c r="E1" s="111"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
       <c r="F1" s="41"/>
       <c r="G1" s="41"/>
       <c r="H1" s="41"/>
@@ -4735,13 +4735,13 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="112" t="s">
+      <c r="A2" s="116" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="112"/>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
+      <c r="B2" s="116"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
       <c r="F2" s="44"/>
       <c r="G2" s="44"/>
       <c r="H2" s="44"/>
@@ -4752,13 +4752,13 @@
       <c r="M2" s="44"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="114" t="s">
+      <c r="A3" s="118" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="114"/>
-      <c r="C3" s="114"/>
-      <c r="D3" s="114"/>
-      <c r="E3" s="114"/>
+      <c r="B3" s="118"/>
+      <c r="C3" s="118"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
       <c r="F3" s="46"/>
       <c r="G3" s="46"/>
       <c r="H3" s="46"/>
@@ -4769,11 +4769,11 @@
       <c r="M3" s="46"/>
     </row>
     <row r="4" spans="1:13" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="113" t="s">
+      <c r="A4" s="117" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="113"/>
-      <c r="C4" s="113"/>
+      <c r="B4" s="117"/>
+      <c r="C4" s="117"/>
       <c r="D4" s="97" t="s">
         <v>40</v>
       </c>
@@ -4850,68 +4850,68 @@
     </row>
     <row r="6" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="122"/>
-      <c r="B6" s="115" t="str">
+      <c r="B6" s="109" t="str">
         <f>Liabilities!B6</f>
         <v>Audited</v>
       </c>
-      <c r="C6" s="115" t="str">
+      <c r="C6" s="109" t="str">
         <f>Liabilities!C6</f>
         <v>Audited</v>
       </c>
-      <c r="D6" s="115" t="str">
+      <c r="D6" s="109" t="str">
         <f>Liabilities!D6</f>
         <v>Audited</v>
       </c>
-      <c r="E6" s="115" t="str">
+      <c r="E6" s="109" t="str">
         <f>Liabilities!E6</f>
         <v>Estimated</v>
       </c>
-      <c r="F6" s="115" t="e">
+      <c r="F6" s="109" t="e">
         <f>Liabilities!F6</f>
         <v>#REF!</v>
       </c>
-      <c r="G6" s="115" t="e">
+      <c r="G6" s="109" t="e">
         <f>Liabilities!G6</f>
         <v>#REF!</v>
       </c>
-      <c r="H6" s="115" t="e">
+      <c r="H6" s="109" t="e">
         <f>Liabilities!H6</f>
         <v>#REF!</v>
       </c>
-      <c r="I6" s="115" t="e">
+      <c r="I6" s="109" t="e">
         <f>Liabilities!I6</f>
         <v>#REF!</v>
       </c>
-      <c r="J6" s="115" t="e">
+      <c r="J6" s="109" t="e">
         <f>Liabilities!J6</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="115" t="e">
+      <c r="K6" s="109" t="e">
         <f>Liabilities!K6</f>
         <v>#REF!</v>
       </c>
-      <c r="L6" s="115" t="e">
+      <c r="L6" s="109" t="e">
         <f>Liabilities!L6</f>
         <v>#REF!</v>
       </c>
-      <c r="M6" s="117" t="e">
+      <c r="M6" s="107" t="e">
         <f>Liabilities!M6</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="122"/>
-      <c r="B7" s="116"/>
-      <c r="C7" s="116"/>
-      <c r="D7" s="116"/>
-      <c r="E7" s="116"/>
-      <c r="F7" s="116"/>
-      <c r="G7" s="116"/>
-      <c r="H7" s="116"/>
-      <c r="I7" s="116"/>
-      <c r="J7" s="116"/>
-      <c r="K7" s="116"/>
-      <c r="L7" s="116"/>
+      <c r="B7" s="119"/>
+      <c r="C7" s="119"/>
+      <c r="D7" s="119"/>
+      <c r="E7" s="119"/>
+      <c r="F7" s="119"/>
+      <c r="G7" s="119"/>
+      <c r="H7" s="119"/>
+      <c r="I7" s="119"/>
+      <c r="J7" s="119"/>
+      <c r="K7" s="119"/>
+      <c r="L7" s="119"/>
       <c r="M7" s="120"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -5375,10 +5375,10 @@
       <c r="A29" s="79" t="s">
         <v>88</v>
       </c>
-      <c r="B29" s="82"/>
-      <c r="C29" s="82"/>
-      <c r="D29" s="82"/>
-      <c r="E29" s="82"/>
+      <c r="B29" s="80"/>
+      <c r="C29" s="80"/>
+      <c r="D29" s="80"/>
+      <c r="E29" s="5"/>
       <c r="F29" s="82" t="e">
         <f>'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
@@ -5431,10 +5431,10 @@
       <c r="A31" s="79" t="s">
         <v>87</v>
       </c>
-      <c r="B31" s="82"/>
-      <c r="C31" s="82"/>
-      <c r="D31" s="82"/>
-      <c r="E31" s="82"/>
+      <c r="B31" s="80"/>
+      <c r="C31" s="80"/>
+      <c r="D31" s="80"/>
+      <c r="E31" s="5"/>
       <c r="F31" s="82" t="e">
         <f>'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
@@ -7087,6 +7087,7 @@
   </sheetData>
   <sheetProtection password="CF53" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="17">
+    <mergeCell ref="L6:L7"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A3:E3"/>
@@ -7103,7 +7104,6 @@
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="50" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ntb primary view changes
</commit_message>
<xml_diff>
--- a/service-loans/template/Template_CW_CMA.xlsx
+++ b/service-loans/template/Template_CW_CMA.xlsx
@@ -1389,6 +1389,18 @@
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -1417,19 +1429,7 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2827,13 +2827,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="115" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="111"/>
-      <c r="C1" s="111"/>
-      <c r="D1" s="111"/>
-      <c r="E1" s="111"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
       <c r="F1" s="40"/>
       <c r="G1" s="41"/>
       <c r="H1" s="41"/>
@@ -2854,13 +2854,13 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="112" t="s">
+      <c r="A2" s="116" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="112"/>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
+      <c r="B2" s="116"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
       <c r="F2" s="44"/>
       <c r="G2" s="44"/>
       <c r="H2" s="44"/>
@@ -2871,13 +2871,13 @@
       <c r="M2" s="44"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="114" t="s">
+      <c r="A3" s="118" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="114"/>
-      <c r="C3" s="114"/>
-      <c r="D3" s="114"/>
-      <c r="E3" s="114"/>
+      <c r="B3" s="118"/>
+      <c r="C3" s="118"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
       <c r="F3" s="46"/>
       <c r="G3" s="46"/>
       <c r="H3" s="46"/>
@@ -2888,11 +2888,11 @@
       <c r="M3" s="46"/>
     </row>
     <row r="4" spans="1:13" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="113" t="s">
+      <c r="A4" s="117" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="113"/>
-      <c r="C4" s="113"/>
+      <c r="B4" s="117"/>
+      <c r="C4" s="117"/>
       <c r="D4" s="97" t="s">
         <v>40</v>
       </c>
@@ -2915,7 +2915,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="109" t="s">
+      <c r="A5" s="113" t="s">
         <v>71</v>
       </c>
       <c r="B5" s="28">
@@ -2968,70 +2968,70 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="110"/>
-      <c r="B6" s="115" t="str">
+      <c r="A6" s="114"/>
+      <c r="B6" s="109" t="str">
         <f>+'Operating Stmt.'!B6:B6</f>
         <v>Audited</v>
       </c>
-      <c r="C6" s="115" t="str">
+      <c r="C6" s="109" t="str">
         <f>+'Operating Stmt.'!C6:C6</f>
         <v>Audited</v>
       </c>
-      <c r="D6" s="115" t="str">
+      <c r="D6" s="109" t="str">
         <f>+'Operating Stmt.'!D6:D6</f>
         <v>Audited</v>
       </c>
-      <c r="E6" s="115" t="str">
+      <c r="E6" s="109" t="str">
         <f>+'Operating Stmt.'!E6:E6</f>
         <v>Estimated</v>
       </c>
-      <c r="F6" s="115" t="e">
+      <c r="F6" s="109" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="G6" s="115" t="e">
+      <c r="G6" s="109" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="H6" s="115" t="e">
+      <c r="H6" s="109" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="I6" s="115" t="e">
+      <c r="I6" s="109" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="J6" s="115" t="e">
+      <c r="J6" s="109" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="115" t="e">
+      <c r="K6" s="109" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="L6" s="115" t="e">
+      <c r="L6" s="109" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="M6" s="117" t="e">
+      <c r="M6" s="107" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="110"/>
-      <c r="B7" s="116"/>
-      <c r="C7" s="116"/>
-      <c r="D7" s="116"/>
-      <c r="E7" s="116"/>
-      <c r="F7" s="119"/>
-      <c r="G7" s="119"/>
-      <c r="H7" s="119"/>
-      <c r="I7" s="119"/>
-      <c r="J7" s="119"/>
-      <c r="K7" s="119"/>
-      <c r="L7" s="119"/>
-      <c r="M7" s="118"/>
+      <c r="A7" s="114"/>
+      <c r="B7" s="119"/>
+      <c r="C7" s="119"/>
+      <c r="D7" s="119"/>
+      <c r="E7" s="119"/>
+      <c r="F7" s="110"/>
+      <c r="G7" s="110"/>
+      <c r="H7" s="110"/>
+      <c r="I7" s="110"/>
+      <c r="J7" s="110"/>
+      <c r="K7" s="110"/>
+      <c r="L7" s="110"/>
+      <c r="M7" s="108"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="53" t="s">
@@ -3477,7 +3477,7 @@
       <c r="M32" s="3"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="107"/>
+      <c r="A33" s="111"/>
       <c r="B33" s="55"/>
       <c r="C33" s="55"/>
       <c r="D33" s="55"/>
@@ -3492,7 +3492,7 @@
       <c r="M33" s="3"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="108"/>
+      <c r="A34" s="112"/>
       <c r="B34" s="55"/>
       <c r="C34" s="55"/>
       <c r="D34" s="55"/>
@@ -4655,14 +4655,6 @@
   </sheetData>
   <sheetProtection password="CF53" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="18">
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="H6:H7"/>
     <mergeCell ref="A33:A34"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="A1:E1"/>
@@ -4673,6 +4665,14 @@
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="H6:H7"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:M13 B17:M32 B82:M83 B41:M53 B67:M80 B57:M57">
@@ -4708,13 +4708,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="115" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="111"/>
-      <c r="C1" s="111"/>
-      <c r="D1" s="111"/>
-      <c r="E1" s="111"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
       <c r="F1" s="41"/>
       <c r="G1" s="41"/>
       <c r="H1" s="41"/>
@@ -4735,13 +4735,13 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="112" t="s">
+      <c r="A2" s="116" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="112"/>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
+      <c r="B2" s="116"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
       <c r="F2" s="44"/>
       <c r="G2" s="44"/>
       <c r="H2" s="44"/>
@@ -4752,13 +4752,13 @@
       <c r="M2" s="44"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="114" t="s">
+      <c r="A3" s="118" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="114"/>
-      <c r="C3" s="114"/>
-      <c r="D3" s="114"/>
-      <c r="E3" s="114"/>
+      <c r="B3" s="118"/>
+      <c r="C3" s="118"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
       <c r="F3" s="46"/>
       <c r="G3" s="46"/>
       <c r="H3" s="46"/>
@@ -4769,11 +4769,11 @@
       <c r="M3" s="46"/>
     </row>
     <row r="4" spans="1:13" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="113" t="s">
+      <c r="A4" s="117" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="113"/>
-      <c r="C4" s="113"/>
+      <c r="B4" s="117"/>
+      <c r="C4" s="117"/>
       <c r="D4" s="97" t="s">
         <v>40</v>
       </c>
@@ -4850,68 +4850,68 @@
     </row>
     <row r="6" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="122"/>
-      <c r="B6" s="115" t="str">
+      <c r="B6" s="109" t="str">
         <f>Liabilities!B6</f>
         <v>Audited</v>
       </c>
-      <c r="C6" s="115" t="str">
+      <c r="C6" s="109" t="str">
         <f>Liabilities!C6</f>
         <v>Audited</v>
       </c>
-      <c r="D6" s="115" t="str">
+      <c r="D6" s="109" t="str">
         <f>Liabilities!D6</f>
         <v>Audited</v>
       </c>
-      <c r="E6" s="115" t="str">
+      <c r="E6" s="109" t="str">
         <f>Liabilities!E6</f>
         <v>Estimated</v>
       </c>
-      <c r="F6" s="115" t="e">
+      <c r="F6" s="109" t="e">
         <f>Liabilities!F6</f>
         <v>#REF!</v>
       </c>
-      <c r="G6" s="115" t="e">
+      <c r="G6" s="109" t="e">
         <f>Liabilities!G6</f>
         <v>#REF!</v>
       </c>
-      <c r="H6" s="115" t="e">
+      <c r="H6" s="109" t="e">
         <f>Liabilities!H6</f>
         <v>#REF!</v>
       </c>
-      <c r="I6" s="115" t="e">
+      <c r="I6" s="109" t="e">
         <f>Liabilities!I6</f>
         <v>#REF!</v>
       </c>
-      <c r="J6" s="115" t="e">
+      <c r="J6" s="109" t="e">
         <f>Liabilities!J6</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="115" t="e">
+      <c r="K6" s="109" t="e">
         <f>Liabilities!K6</f>
         <v>#REF!</v>
       </c>
-      <c r="L6" s="115" t="e">
+      <c r="L6" s="109" t="e">
         <f>Liabilities!L6</f>
         <v>#REF!</v>
       </c>
-      <c r="M6" s="117" t="e">
+      <c r="M6" s="107" t="e">
         <f>Liabilities!M6</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="122"/>
-      <c r="B7" s="116"/>
-      <c r="C7" s="116"/>
-      <c r="D7" s="116"/>
-      <c r="E7" s="116"/>
-      <c r="F7" s="116"/>
-      <c r="G7" s="116"/>
-      <c r="H7" s="116"/>
-      <c r="I7" s="116"/>
-      <c r="J7" s="116"/>
-      <c r="K7" s="116"/>
-      <c r="L7" s="116"/>
+      <c r="B7" s="119"/>
+      <c r="C7" s="119"/>
+      <c r="D7" s="119"/>
+      <c r="E7" s="119"/>
+      <c r="F7" s="119"/>
+      <c r="G7" s="119"/>
+      <c r="H7" s="119"/>
+      <c r="I7" s="119"/>
+      <c r="J7" s="119"/>
+      <c r="K7" s="119"/>
+      <c r="L7" s="119"/>
       <c r="M7" s="120"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -5375,10 +5375,10 @@
       <c r="A29" s="79" t="s">
         <v>88</v>
       </c>
-      <c r="B29" s="82"/>
-      <c r="C29" s="82"/>
-      <c r="D29" s="82"/>
-      <c r="E29" s="82"/>
+      <c r="B29" s="80"/>
+      <c r="C29" s="80"/>
+      <c r="D29" s="80"/>
+      <c r="E29" s="5"/>
       <c r="F29" s="82" t="e">
         <f>'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
@@ -5431,10 +5431,10 @@
       <c r="A31" s="79" t="s">
         <v>87</v>
       </c>
-      <c r="B31" s="82"/>
-      <c r="C31" s="82"/>
-      <c r="D31" s="82"/>
-      <c r="E31" s="82"/>
+      <c r="B31" s="80"/>
+      <c r="C31" s="80"/>
+      <c r="D31" s="80"/>
+      <c r="E31" s="5"/>
       <c r="F31" s="82" t="e">
         <f>'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
@@ -7087,6 +7087,7 @@
   </sheetData>
   <sheetProtection password="CF53" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="17">
+    <mergeCell ref="L6:L7"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A3:E3"/>
@@ -7103,7 +7104,6 @@
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="50" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
cma changes and ntb code changes
</commit_message>
<xml_diff>
--- a/service-loans/template/Template_CW_CMA.xlsx
+++ b/service-loans/template/Template_CW_CMA.xlsx
@@ -1,18 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC49F3CD-D6C1-47E7-AF67-2A27D17CACB9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="nMIDBcyH02QIBA4bXtkulhW+BkwLjO6uUdnHuLe/vey9rIzKWc8NDkCsYZON8UKSky/yikEzYHsiuF6pBe7KDg==" workbookSaltValue="OCFZwCBGKUImSpaXHpKcuQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operating Stmt." sheetId="2" r:id="rId1"/>
     <sheet name="Liabilities" sheetId="3" r:id="rId2"/>
     <sheet name="Asset" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -100,9 +108,6 @@
     <t xml:space="preserve">     i]  Raw materials[including stores     &amp; other items used in the process of manufacture]</t>
   </si>
   <si>
-    <t>5.  Cost of Sales</t>
-  </si>
-  <si>
     <t>4.  % rise [+] or fall [-]in net sales as compared to last year [annualised]</t>
   </si>
   <si>
@@ -110,9 +115,6 @@
   </si>
   <si>
     <t xml:space="preserve">   Deduct other items</t>
-  </si>
-  <si>
-    <t>2. Less Excise Duty</t>
   </si>
   <si>
     <t xml:space="preserve">     Total</t>
@@ -554,11 +556,17 @@
   <si>
     <t>Other Assets (Need to check at the time of Due Diligence)</t>
   </si>
+  <si>
+    <t>2. Less : Indirect Taxes</t>
+  </si>
+  <si>
+    <t>5.  Cost of Sales (including indirect taxes)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
@@ -1389,18 +1397,6 @@
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -1429,7 +1425,19 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1444,7 +1452,7 @@
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="4" builtinId="3"/>
-    <cellStyle name="Comma 2" xfId="2"/>
+    <cellStyle name="Comma 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
@@ -1505,7 +1513,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1538,9 +1546,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1573,6 +1598,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1748,7 +1790,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -1756,7 +1798,7 @@
       <selection activeCell="B67" sqref="B67"/>
       <selection pane="topRight" activeCell="B67" sqref="B67"/>
       <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1773,43 +1815,43 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="102" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B1" s="102"/>
       <c r="C1" s="102"/>
       <c r="D1" s="102"/>
       <c r="E1" s="102"/>
       <c r="F1" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I1" s="19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J1" s="19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="103" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B2" s="103"/>
       <c r="C2" s="103"/>
       <c r="D2" s="103"/>
       <c r="E2" s="103"/>
       <c r="F2" s="19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="104" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" s="104"/>
       <c r="C3" s="104"/>
@@ -1818,15 +1860,15 @@
     </row>
     <row r="4" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="105" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B4" s="106"/>
       <c r="C4" s="106"/>
       <c r="D4" s="97" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E4" s="98" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
@@ -1850,21 +1892,21 @@
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B7" s="29"/>
       <c r="C7" s="29"/>
@@ -1875,7 +1917,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B8" s="30"/>
       <c r="C8" s="30"/>
@@ -1886,7 +1928,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B9" s="30"/>
       <c r="C9" s="30"/>
@@ -1897,7 +1939,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B10" s="30"/>
       <c r="C10" s="30"/>
@@ -1908,7 +1950,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B11" s="31">
         <f>SUM(ROUND(B8+B9+B10,2))</f>
@@ -1940,7 +1982,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
-        <v>31</v>
+        <v>169</v>
       </c>
       <c r="B13" s="30"/>
       <c r="C13" s="30"/>
@@ -1949,7 +1991,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="30"/>
       <c r="C14" s="30"/>
@@ -1958,7 +2000,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="31">
         <f t="shared" ref="B15:E15" si="1">IF(B11=0,0,SUM(ROUND((B11)-(B13+B14),2)))</f>
@@ -1986,7 +2028,7 @@
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" s="31"/>
       <c r="C17" s="33">
@@ -2011,7 +2053,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
-        <v>27</v>
+        <v>170</v>
       </c>
       <c r="B19" s="32"/>
       <c r="C19" s="32"/>
@@ -2380,7 +2422,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B54" s="34"/>
       <c r="C54" s="34"/>
@@ -2396,7 +2438,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="24" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B56" s="37"/>
       <c r="C56" s="37"/>
@@ -2412,7 +2454,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B58" s="38">
         <f>(ROUND(B52+B56+B54,2))</f>
@@ -2440,7 +2482,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="24" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B60" s="38">
         <f t="shared" ref="B60:E60" si="11">IF(B58&lt;0,(ROUND(B15+B58,2)),(ROUND(B15-B58,2)))</f>
@@ -2468,7 +2510,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="24" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B62" s="11"/>
       <c r="C62" s="11"/>
@@ -2484,7 +2526,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="24" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B64" s="38">
         <f t="shared" ref="B64:E64" si="12">(ROUND(B60-B62,2))</f>
@@ -2512,7 +2554,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="24" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B66" s="11"/>
       <c r="C66" s="11"/>
@@ -2609,7 +2651,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="24" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B73" s="38">
         <f t="shared" ref="B73:E73" si="16">SUM(ROUND(B64+B70-B71,2))</f>
@@ -2637,7 +2679,7 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="24" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B75" s="11"/>
       <c r="C75" s="11"/>
@@ -2646,7 +2688,7 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="99" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B76" s="11"/>
       <c r="C76" s="11"/>
@@ -2696,7 +2738,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="24" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B80" s="12"/>
       <c r="C80" s="11"/>
@@ -2740,7 +2782,7 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="24" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B84" s="38">
         <f t="shared" ref="B84:E84" si="18">B78-B80</f>
@@ -2768,7 +2810,7 @@
     </row>
     <row r="86" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="27" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B86" s="39">
         <f t="shared" ref="B86:E86" si="19">IFERROR((B84/B78),0)</f>
@@ -2788,7 +2830,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="CF53" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="4">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
@@ -2796,10 +2838,10 @@
     <mergeCell ref="A4:C4"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:E16 B18:E81">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:E16 B18:E81" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82:E86 B17:E17"/>
+    <dataValidation operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82:E86 B17:E17" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2807,11 +2849,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M87"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="7" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B67" sqref="B67"/>
       <selection pane="topRight" activeCell="B67" sqref="B67"/>
       <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
@@ -2827,40 +2869,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="115" t="s">
-        <v>74</v>
-      </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
+      <c r="A1" s="111" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="111"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
       <c r="F1" s="40"/>
       <c r="G1" s="41"/>
       <c r="H1" s="41"/>
       <c r="I1" s="42" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J1" s="42" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="K1" s="42" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="L1" s="43" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M1" s="43" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="116" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" s="116"/>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
+      <c r="A2" s="112" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="112"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
       <c r="F2" s="44"/>
       <c r="G2" s="44"/>
       <c r="H2" s="44"/>
@@ -2871,13 +2913,13 @@
       <c r="M2" s="44"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="118" t="s">
-        <v>72</v>
-      </c>
-      <c r="B3" s="118"/>
-      <c r="C3" s="118"/>
-      <c r="D3" s="118"/>
-      <c r="E3" s="118"/>
+      <c r="A3" s="114" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="114"/>
+      <c r="C3" s="114"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="114"/>
       <c r="F3" s="46"/>
       <c r="G3" s="46"/>
       <c r="H3" s="46"/>
@@ -2888,16 +2930,16 @@
       <c r="M3" s="46"/>
     </row>
     <row r="4" spans="1:13" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="117" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="117"/>
-      <c r="C4" s="117"/>
+      <c r="A4" s="113" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="113"/>
+      <c r="C4" s="113"/>
       <c r="D4" s="97" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E4" s="98" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F4" s="47"/>
       <c r="G4" s="47"/>
@@ -2915,8 +2957,8 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="113" t="s">
-        <v>71</v>
+      <c r="A5" s="109" t="s">
+        <v>69</v>
       </c>
       <c r="B5" s="28">
         <f>'Operating Stmt.'!B5</f>
@@ -2968,74 +3010,74 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="114"/>
-      <c r="B6" s="109" t="str">
+      <c r="A6" s="110"/>
+      <c r="B6" s="115" t="str">
         <f>+'Operating Stmt.'!B6:B6</f>
         <v>Audited</v>
       </c>
-      <c r="C6" s="109" t="str">
+      <c r="C6" s="115" t="str">
         <f>+'Operating Stmt.'!C6:C6</f>
         <v>Audited</v>
       </c>
-      <c r="D6" s="109" t="str">
+      <c r="D6" s="115" t="str">
         <f>+'Operating Stmt.'!D6:D6</f>
         <v>Audited</v>
       </c>
-      <c r="E6" s="109" t="str">
+      <c r="E6" s="115" t="str">
         <f>+'Operating Stmt.'!E6:E6</f>
         <v>Estimated</v>
       </c>
-      <c r="F6" s="109" t="e">
+      <c r="F6" s="115" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="G6" s="109" t="e">
+      <c r="G6" s="115" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="H6" s="109" t="e">
+      <c r="H6" s="115" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="I6" s="109" t="e">
+      <c r="I6" s="115" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="J6" s="109" t="e">
+      <c r="J6" s="115" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="109" t="e">
+      <c r="K6" s="115" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="L6" s="109" t="e">
+      <c r="L6" s="115" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="M6" s="107" t="e">
+      <c r="M6" s="117" t="e">
         <f>+'Operating Stmt.'!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="114"/>
-      <c r="B7" s="119"/>
-      <c r="C7" s="119"/>
-      <c r="D7" s="119"/>
-      <c r="E7" s="119"/>
-      <c r="F7" s="110"/>
-      <c r="G7" s="110"/>
-      <c r="H7" s="110"/>
-      <c r="I7" s="110"/>
-      <c r="J7" s="110"/>
-      <c r="K7" s="110"/>
-      <c r="L7" s="110"/>
-      <c r="M7" s="108"/>
+      <c r="A7" s="110"/>
+      <c r="B7" s="116"/>
+      <c r="C7" s="116"/>
+      <c r="D7" s="116"/>
+      <c r="E7" s="116"/>
+      <c r="F7" s="119"/>
+      <c r="G7" s="119"/>
+      <c r="H7" s="119"/>
+      <c r="I7" s="119"/>
+      <c r="J7" s="119"/>
+      <c r="K7" s="119"/>
+      <c r="L7" s="119"/>
+      <c r="M7" s="118"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="53" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B8" s="54"/>
       <c r="C8" s="54"/>
@@ -3052,7 +3094,7 @@
     </row>
     <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B9" s="55"/>
       <c r="C9" s="55"/>
@@ -3086,7 +3128,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B11" s="56"/>
       <c r="C11" s="56"/>
@@ -3103,7 +3145,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B12" s="56"/>
       <c r="C12" s="56"/>
@@ -3120,7 +3162,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B13" s="56"/>
       <c r="C13" s="56"/>
@@ -3137,7 +3179,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B14" s="55"/>
       <c r="C14" s="55"/>
@@ -3154,7 +3196,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B15" s="57">
         <f>SUM(ROUND(B11+B12,2))</f>
@@ -3222,7 +3264,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B17" s="56"/>
       <c r="C17" s="56"/>
@@ -3254,7 +3296,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B19" s="55"/>
       <c r="C19" s="55"/>
@@ -3286,7 +3328,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="26" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B21" s="56"/>
       <c r="C21" s="56"/>
@@ -3318,7 +3360,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B23" s="56"/>
       <c r="C23" s="56"/>
@@ -3350,7 +3392,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B25" s="56"/>
       <c r="C25" s="56"/>
@@ -3382,7 +3424,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="26" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B27" s="56"/>
       <c r="C27" s="56"/>
@@ -3414,7 +3456,7 @@
     </row>
     <row r="29" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="58" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B29" s="56"/>
       <c r="C29" s="56"/>
@@ -3461,7 +3503,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="59" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B32" s="60"/>
       <c r="C32" s="56"/>
@@ -3477,7 +3519,7 @@
       <c r="M32" s="3"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="111"/>
+      <c r="A33" s="107"/>
       <c r="B33" s="55"/>
       <c r="C33" s="55"/>
       <c r="D33" s="55"/>
@@ -3492,7 +3534,7 @@
       <c r="M33" s="3"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="112"/>
+      <c r="A34" s="108"/>
       <c r="B34" s="55"/>
       <c r="C34" s="55"/>
       <c r="D34" s="55"/>
@@ -3508,7 +3550,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="61" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B35" s="57">
         <f t="shared" ref="B35:M35" si="1">SUM(ROUND(B17+B19+B21+B23+B25+B27+B29+B32,2))</f>
@@ -3576,7 +3618,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="62" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B37" s="57">
         <f t="shared" ref="B37:M37" si="2">SUM(ROUND(B15+B35,2))</f>
@@ -3644,7 +3686,7 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="65" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B39" s="55"/>
       <c r="C39" s="55"/>
@@ -3676,7 +3718,7 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="24" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B41" s="56"/>
       <c r="C41" s="56"/>
@@ -3708,7 +3750,7 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="26" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B43" s="56"/>
       <c r="C43" s="56"/>
@@ -3740,7 +3782,7 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B45" s="56">
         <f>SUM(ROUND(B46+B47,2))</f>
@@ -3793,7 +3835,7 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="66" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B46" s="56"/>
       <c r="C46" s="56"/>
@@ -3810,7 +3852,7 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="66" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B47" s="56"/>
       <c r="C47" s="56"/>
@@ -3842,7 +3884,7 @@
     </row>
     <row r="49" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B49" s="56"/>
       <c r="C49" s="56"/>
@@ -3859,7 +3901,7 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B50" s="55"/>
       <c r="C50" s="55"/>
@@ -3876,7 +3918,7 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="24" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B51" s="56"/>
       <c r="C51" s="56"/>
@@ -3908,7 +3950,7 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="24" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B53" s="56"/>
       <c r="C53" s="56"/>
@@ -3940,7 +3982,7 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="67" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B55" s="57">
         <f t="shared" ref="B55:M55" si="4">SUM(ROUND(B41+B43+B45+B49+B51+B53,2))</f>
@@ -4008,7 +4050,7 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="67" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B57" s="100">
         <f>SUM(ROUND(B58+B59+B60+B61,2))</f>
@@ -4061,7 +4103,7 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="68" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B58" s="57"/>
       <c r="C58" s="57"/>
@@ -4078,7 +4120,7 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="68" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B59" s="57"/>
       <c r="C59" s="57"/>
@@ -4095,7 +4137,7 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="68" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B60" s="57"/>
       <c r="C60" s="57"/>
@@ -4112,7 +4154,7 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="68" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B61" s="57"/>
       <c r="C61" s="57"/>
@@ -4143,7 +4185,7 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="69" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B63" s="101">
         <f>SUM(ROUND(B37+B55+B57,2))</f>
@@ -4211,7 +4253,7 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="53" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B65" s="55"/>
       <c r="C65" s="55"/>
@@ -4243,7 +4285,7 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B67" s="56"/>
       <c r="C67" s="56"/>
@@ -4275,7 +4317,7 @@
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="24" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B69" s="56"/>
       <c r="C69" s="56"/>
@@ -4307,7 +4349,7 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="24" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B71" s="55"/>
       <c r="C71" s="55"/>
@@ -4339,7 +4381,7 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="24" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B73" s="56"/>
       <c r="C73" s="56"/>
@@ -4371,7 +4413,7 @@
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="24" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B75" s="56"/>
       <c r="C75" s="56"/>
@@ -4403,7 +4445,7 @@
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="24" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B77" s="56"/>
       <c r="C77" s="56"/>
@@ -4435,7 +4477,7 @@
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="26" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B79" s="56"/>
       <c r="C79" s="56"/>
@@ -4467,7 +4509,7 @@
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="24" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B81" s="55"/>
       <c r="C81" s="55"/>
@@ -4499,7 +4541,7 @@
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="24" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B83" s="55"/>
       <c r="C83" s="55"/>
@@ -4531,7 +4573,7 @@
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="24" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B85" s="57">
         <f>SUM(ROUND(B67+B69+B71+B73+B75+B77+B79+B81+B83,2))</f>
@@ -4584,7 +4626,7 @@
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="99" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B86" s="55"/>
       <c r="C86" s="55"/>
@@ -4601,7 +4643,7 @@
     </row>
     <row r="87" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="70" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B87" s="71">
         <f>SUM(ROUND(B63+B85+B86,2))</f>
@@ -4655,6 +4697,14 @@
   </sheetData>
   <sheetProtection password="CF53" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="18">
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="H6:H7"/>
     <mergeCell ref="A33:A34"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="A1:E1"/>
@@ -4665,20 +4715,12 @@
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="H6:H7"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:M13 B17:M32 B82:M83 B41:M53 B67:M80 B57:M57">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:M13 B17:M32 B82:M83 B41:M53 B67:M80 B57:M57" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B81:M81">
+    <dataValidation type="whole" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B81:M81" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>1E+35</formula1>
     </dataValidation>
   </dataValidations>
@@ -4688,7 +4730,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M99"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -4708,40 +4750,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="115" t="s">
-        <v>96</v>
-      </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
+      <c r="A1" s="111" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="111"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
       <c r="F1" s="41"/>
       <c r="G1" s="41"/>
       <c r="H1" s="41"/>
       <c r="I1" s="42" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J1" s="42" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="K1" s="42" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="L1" s="43" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M1" s="43" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="116" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" s="116"/>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
+      <c r="A2" s="112" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="112"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
       <c r="F2" s="44"/>
       <c r="G2" s="44"/>
       <c r="H2" s="44"/>
@@ -4752,13 +4794,13 @@
       <c r="M2" s="44"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="118" t="s">
-        <v>72</v>
-      </c>
-      <c r="B3" s="118"/>
-      <c r="C3" s="118"/>
-      <c r="D3" s="118"/>
-      <c r="E3" s="118"/>
+      <c r="A3" s="114" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="114"/>
+      <c r="C3" s="114"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="114"/>
       <c r="F3" s="46"/>
       <c r="G3" s="46"/>
       <c r="H3" s="46"/>
@@ -4769,16 +4811,16 @@
       <c r="M3" s="46"/>
     </row>
     <row r="4" spans="1:13" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="117" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="117"/>
-      <c r="C4" s="117"/>
+      <c r="A4" s="113" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="113"/>
+      <c r="C4" s="113"/>
       <c r="D4" s="97" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E4" s="98" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F4" s="47"/>
       <c r="G4" s="47"/>
@@ -4797,7 +4839,7 @@
     </row>
     <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A5" s="121" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B5" s="75">
         <f>'Operating Stmt.'!B5</f>
@@ -4850,73 +4892,73 @@
     </row>
     <row r="6" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="122"/>
-      <c r="B6" s="109" t="str">
+      <c r="B6" s="115" t="str">
         <f>Liabilities!B6</f>
         <v>Audited</v>
       </c>
-      <c r="C6" s="109" t="str">
+      <c r="C6" s="115" t="str">
         <f>Liabilities!C6</f>
         <v>Audited</v>
       </c>
-      <c r="D6" s="109" t="str">
+      <c r="D6" s="115" t="str">
         <f>Liabilities!D6</f>
         <v>Audited</v>
       </c>
-      <c r="E6" s="109" t="str">
+      <c r="E6" s="115" t="str">
         <f>Liabilities!E6</f>
         <v>Estimated</v>
       </c>
-      <c r="F6" s="109" t="e">
+      <c r="F6" s="115" t="e">
         <f>Liabilities!F6</f>
         <v>#REF!</v>
       </c>
-      <c r="G6" s="109" t="e">
+      <c r="G6" s="115" t="e">
         <f>Liabilities!G6</f>
         <v>#REF!</v>
       </c>
-      <c r="H6" s="109" t="e">
+      <c r="H6" s="115" t="e">
         <f>Liabilities!H6</f>
         <v>#REF!</v>
       </c>
-      <c r="I6" s="109" t="e">
+      <c r="I6" s="115" t="e">
         <f>Liabilities!I6</f>
         <v>#REF!</v>
       </c>
-      <c r="J6" s="109" t="e">
+      <c r="J6" s="115" t="e">
         <f>Liabilities!J6</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="109" t="e">
+      <c r="K6" s="115" t="e">
         <f>Liabilities!K6</f>
         <v>#REF!</v>
       </c>
-      <c r="L6" s="109" t="e">
+      <c r="L6" s="115" t="e">
         <f>Liabilities!L6</f>
         <v>#REF!</v>
       </c>
-      <c r="M6" s="107" t="e">
+      <c r="M6" s="117" t="e">
         <f>Liabilities!M6</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="122"/>
-      <c r="B7" s="119"/>
-      <c r="C7" s="119"/>
-      <c r="D7" s="119"/>
-      <c r="E7" s="119"/>
-      <c r="F7" s="119"/>
-      <c r="G7" s="119"/>
-      <c r="H7" s="119"/>
-      <c r="I7" s="119"/>
-      <c r="J7" s="119"/>
-      <c r="K7" s="119"/>
-      <c r="L7" s="119"/>
+      <c r="B7" s="116"/>
+      <c r="C7" s="116"/>
+      <c r="D7" s="116"/>
+      <c r="E7" s="116"/>
+      <c r="F7" s="116"/>
+      <c r="G7" s="116"/>
+      <c r="H7" s="116"/>
+      <c r="I7" s="116"/>
+      <c r="J7" s="116"/>
+      <c r="K7" s="116"/>
+      <c r="L7" s="116"/>
       <c r="M7" s="120"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="76" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B8" s="77"/>
       <c r="C8" s="78"/>
@@ -4933,7 +4975,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="79" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B9" s="80"/>
       <c r="C9" s="55"/>
@@ -4965,7 +5007,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="81" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B11" s="82">
         <f t="shared" ref="B11:M11" si="0">SUM(ROUND(B13+B15,2))</f>
@@ -5018,7 +5060,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="79" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B12" s="80"/>
       <c r="C12" s="55"/>
@@ -5035,7 +5077,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="79" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B13" s="80"/>
       <c r="C13" s="55"/>
@@ -5052,7 +5094,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="79" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B14" s="80"/>
       <c r="C14" s="80"/>
@@ -5069,7 +5111,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="79" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B15" s="80"/>
       <c r="C15" s="55"/>
@@ -5086,7 +5128,7 @@
     </row>
     <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="81" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B16" s="80"/>
       <c r="C16" s="55"/>
@@ -5103,7 +5145,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="79" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B17" s="80"/>
       <c r="C17" s="80"/>
@@ -5120,7 +5162,7 @@
     </row>
     <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="81" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B18" s="80"/>
       <c r="C18" s="55"/>
@@ -5137,7 +5179,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="79" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B19" s="80"/>
       <c r="C19" s="80"/>
@@ -5154,7 +5196,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="81" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B20" s="80"/>
       <c r="C20" s="55"/>
@@ -5186,7 +5228,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="79" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B22" s="82">
         <f t="shared" ref="B22:M22" si="1">SUM(ROUND(B24+B29+B31+B33,2))</f>
@@ -5254,7 +5296,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="79" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B24" s="82">
         <f t="shared" ref="B24:M24" si="2">SUM(ROUND(B26+B27,2))</f>
@@ -5307,7 +5349,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="79" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B25" s="80"/>
       <c r="C25" s="55"/>
@@ -5324,7 +5366,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="79" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B26" s="80"/>
       <c r="C26" s="55"/>
@@ -5341,7 +5383,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="79" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B27" s="80"/>
       <c r="C27" s="55"/>
@@ -5373,7 +5415,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="79" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B29" s="80"/>
       <c r="C29" s="80"/>
@@ -5429,7 +5471,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="79" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B31" s="80"/>
       <c r="C31" s="80"/>
@@ -5485,7 +5527,7 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="79" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B33" s="82">
         <f t="shared" ref="B33:M33" si="3">SUM(ROUND(B34+B35,2))</f>
@@ -5538,7 +5580,7 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="79" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B34" s="80"/>
       <c r="C34" s="55"/>
@@ -5555,7 +5597,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="79" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B35" s="80"/>
       <c r="C35" s="55"/>
@@ -5587,7 +5629,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="81" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B37" s="80"/>
       <c r="C37" s="55"/>
@@ -5604,7 +5646,7 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="79" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B38" s="80"/>
       <c r="C38" s="80"/>
@@ -5621,7 +5663,7 @@
     </row>
     <row r="39" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="79" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B39" s="80"/>
       <c r="C39" s="55"/>
@@ -5653,7 +5695,7 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="81" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B41" s="80"/>
       <c r="C41" s="55"/>
@@ -5685,7 +5727,7 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="79" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B43" s="82">
         <f t="shared" ref="B43:M43" si="4">SUM(ROUND(B9+B11+B16+B18+B20+B22+B37+B39+B41,2))</f>
@@ -5753,7 +5795,7 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="81" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B45" s="80">
         <f>SUM(ROUND(B46+B47+B48+B49+B50,2))</f>
@@ -5806,7 +5848,7 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="84" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B46" s="80"/>
       <c r="C46" s="55"/>
@@ -5823,7 +5865,7 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="84" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B47" s="80"/>
       <c r="C47" s="55"/>
@@ -5885,7 +5927,7 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="79" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B51" s="80"/>
       <c r="C51" s="80"/>
@@ -5902,7 +5944,7 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="79" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B52" s="80"/>
       <c r="C52" s="55"/>
@@ -5934,7 +5976,7 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="79" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B54" s="80"/>
       <c r="C54" s="55"/>
@@ -5966,7 +6008,7 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="79" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B56" s="82">
         <f>SUM(ROUND(B45-B52-B54,2))</f>
@@ -6034,7 +6076,7 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="76" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B58" s="80"/>
       <c r="C58" s="55"/>
@@ -6066,7 +6108,7 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="79" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B60" s="80"/>
       <c r="C60" s="55"/>
@@ -6098,7 +6140,7 @@
     </row>
     <row r="62" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="81" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B62" s="82">
         <f>B64+B65+B67+B69+B71</f>
@@ -6151,7 +6193,7 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="79" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B63" s="80"/>
       <c r="C63" s="55"/>
@@ -6168,7 +6210,7 @@
     </row>
     <row r="64" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="81" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B64" s="80"/>
       <c r="C64" s="55"/>
@@ -6185,7 +6227,7 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="79" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B65" s="80"/>
       <c r="C65" s="55"/>
@@ -6217,7 +6259,7 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="81" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B67" s="80"/>
       <c r="C67" s="55"/>
@@ -6234,7 +6276,7 @@
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="79" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B68" s="80"/>
       <c r="C68" s="80"/>
@@ -6251,7 +6293,7 @@
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="81" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B69" s="80"/>
       <c r="C69" s="55"/>
@@ -6268,7 +6310,7 @@
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="79" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B70" s="80"/>
       <c r="C70" s="80"/>
@@ -6285,7 +6327,7 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="79" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B71" s="60">
         <f>SUM(ROUND(B72+B73+B74,2))</f>
@@ -6338,7 +6380,7 @@
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="85" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B72" s="80"/>
       <c r="C72" s="55"/>
@@ -6355,7 +6397,7 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="85" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B73" s="80"/>
       <c r="C73" s="55"/>
@@ -6372,7 +6414,7 @@
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="85" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B74" s="80"/>
       <c r="C74" s="55"/>
@@ -6404,7 +6446,7 @@
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="79" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B76" s="80"/>
       <c r="C76" s="55"/>
@@ -6438,7 +6480,7 @@
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="81" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B78" s="80"/>
       <c r="C78" s="55"/>
@@ -6470,7 +6512,7 @@
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="86" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B80" s="82">
         <f>SUM(ROUND(B60+B62+B76+B78,2))</f>
@@ -6538,7 +6580,7 @@
     </row>
     <row r="82" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="81" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B82" s="82">
         <f t="shared" ref="B82:M82" si="10">ROUND(B83+B84+B85+B86+B87,2)</f>
@@ -6591,7 +6633,7 @@
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="87" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B83" s="80"/>
       <c r="C83" s="55"/>
@@ -6608,7 +6650,7 @@
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" s="87" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B84" s="80"/>
       <c r="C84" s="55"/>
@@ -6625,7 +6667,7 @@
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="87" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B85" s="80"/>
       <c r="C85" s="55"/>
@@ -6642,7 +6684,7 @@
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="87" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B86" s="80"/>
       <c r="C86" s="55"/>
@@ -6659,7 +6701,7 @@
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" s="87" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B87" s="80"/>
       <c r="C87" s="55"/>
@@ -6676,7 +6718,7 @@
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" s="99" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B88" s="80"/>
       <c r="C88" s="80"/>
@@ -6693,7 +6735,7 @@
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" s="79" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B89" s="82">
         <f>SUM(ROUND(B43+B56+B80+B82+B88,2))</f>
@@ -6761,7 +6803,7 @@
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" s="86" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B91" s="82">
         <f>ROUND(Liabilities!B85-Liabilities!B75-Asset!B82,2)</f>
@@ -6829,7 +6871,7 @@
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" s="79" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B93" s="82">
         <f>SUM(ROUND(Liabilities!B55+Liabilities!B85,2))-(ROUND(B56+B80+B82,2))</f>
@@ -6897,7 +6939,7 @@
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" s="79" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B95" s="82">
         <f>IF(Liabilities!B37=0,0,(ROUND(B43/Liabilities!B37,2)))</f>
@@ -6965,7 +7007,7 @@
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" s="79" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B97" s="82">
         <f>IF(B91=0,0,(ROUND(Liabilities!B63/B91,2)))</f>
@@ -7033,7 +7075,7 @@
     </row>
     <row r="99" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="88" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B99" s="89">
         <f>IF(B91=0,0,(ROUND(Liabilities!B55/B91,2)))</f>
@@ -7087,11 +7129,6 @@
   </sheetData>
   <sheetProtection password="CF53" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="17">
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:C4"/>
     <mergeCell ref="M6:M7"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="B6:B7"/>
@@ -7104,6 +7141,11 @@
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="50" orientation="portrait" r:id="rId1"/>

</xml_diff>